<commit_message>
clean up notebooks a bit and replace cellpy file in example_data.py
</commit_message>
<xml_diff>
--- a/docs/examples/data/out/20210210_FC.xlsx
+++ b/docs/examples/data/out/20210210_FC.xlsx
@@ -486,7 +486,7 @@
       </c>
       <c r="B2" s="4" t="inlineStr">
         <is>
-          <t>20210210_FC_01_cc_03-20210210_FC_01_cc_01-20210210_FC_01_cc_04-20210210_FC_01_cc_02</t>
+          <t>20210210_FC_01_cc_01-20210210_FC_01_cc_04-20210210_FC_01_cc_02-20210210_FC_01_cc_03</t>
         </is>
       </c>
     </row>
@@ -1284,7 +1284,7 @@
       </c>
       <c r="B7" s="4" t="inlineStr">
         <is>
-          <t>fullcell</t>
+          <t>full-cell</t>
         </is>
       </c>
     </row>
@@ -1593,10 +1593,10 @@
         <v>0.003324035819317</v>
       </c>
       <c r="I2" t="n">
-        <v>114.8772087938153</v>
+        <v>87.04946877625018</v>
       </c>
       <c r="J2" t="n">
-        <v>114.8772087938153</v>
+        <v>87.04946877625018</v>
       </c>
       <c r="K2" t="n">
         <v>0.003818559568538</v>
@@ -1607,58 +1607,58 @@
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="n">
-        <v>-0.0004945237492210001</v>
+        <v>0.0004945237492210001</v>
       </c>
       <c r="P2" t="n">
-        <v>-0.0004945237492210001</v>
+        <v>0.0004945237492210001</v>
       </c>
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr"/>
       <c r="S2" t="n">
-        <v>-0.0004945237492210001</v>
+        <v>0.0004945237492210001</v>
       </c>
       <c r="T2" t="n">
-        <v>0.002829512070096</v>
+        <v>0.004313083317759</v>
       </c>
       <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr"/>
       <c r="W2" t="inlineStr"/>
       <c r="X2" t="n">
-        <v>3818.559568538001</v>
+        <v>3182.132973781667</v>
       </c>
       <c r="Y2" t="n">
-        <v>180.83741</v>
+        <v>150.69784</v>
       </c>
       <c r="Z2" t="n">
-        <v>180.47164</v>
+        <v>150.39303</v>
       </c>
       <c r="AA2" t="n">
-        <v>3324.035819317</v>
+        <v>2770.029849430834</v>
       </c>
       <c r="AB2" t="n">
-        <v>3818.559568538</v>
+        <v>3182.132973781667</v>
       </c>
       <c r="AC2" t="n">
-        <v>3818.559568538</v>
+        <v>3182.132973781667</v>
       </c>
       <c r="AD2" t="n">
-        <v>3324.035819317</v>
+        <v>2770.029849430834</v>
       </c>
       <c r="AE2" t="n">
-        <v>-494.5237492210001</v>
+        <v>412.1031243508334</v>
       </c>
       <c r="AF2" t="n">
-        <v>-494.5237492210001</v>
+        <v>412.1031243508334</v>
       </c>
       <c r="AG2" t="inlineStr"/>
       <c r="AH2" t="inlineStr"/>
       <c r="AI2" t="inlineStr"/>
       <c r="AJ2" t="inlineStr"/>
       <c r="AK2" t="n">
-        <v>-494.5237492210001</v>
+        <v>412.1031243508334</v>
       </c>
       <c r="AL2" t="n">
-        <v>2829.512070096</v>
+        <v>3594.236098132501</v>
       </c>
       <c r="AM2" t="n">
         <v>3.324035819317</v>
@@ -1673,20 +1673,20 @@
         <v>3.324035819317</v>
       </c>
       <c r="AQ2" t="n">
-        <v>-0.4945237492210001</v>
+        <v>0.4945237492210001</v>
       </c>
       <c r="AR2" t="n">
-        <v>-0.4945237492210001</v>
+        <v>0.4945237492210001</v>
       </c>
       <c r="AS2" t="inlineStr"/>
       <c r="AT2" t="inlineStr"/>
       <c r="AU2" t="inlineStr"/>
       <c r="AV2" t="inlineStr"/>
       <c r="AW2" t="n">
-        <v>-0.4945237492210001</v>
+        <v>0.4945237492210001</v>
       </c>
       <c r="AX2" t="n">
-        <v>2.829512070096</v>
+        <v>4.313083317759</v>
       </c>
     </row>
     <row r="3">
@@ -1715,10 +1715,10 @@
         <v>0.003234381354196</v>
       </c>
       <c r="I3" t="n">
-        <v>105.8080293184443</v>
+        <v>94.51078584880905</v>
       </c>
       <c r="J3" t="n">
-        <v>220.6852381122596</v>
+        <v>181.5602546250592</v>
       </c>
       <c r="K3" t="n">
         <v>0.007240794740056</v>
@@ -1733,10 +1733,10 @@
         <v>0.0003963243970200002</v>
       </c>
       <c r="O3" t="n">
-        <v>-0.000187853817322</v>
+        <v>0.000187853817322</v>
       </c>
       <c r="P3" t="n">
-        <v>-0.0006823775665430001</v>
+        <v>0.0006823775665430001</v>
       </c>
       <c r="Q3" t="n">
         <v>8.965446512100008e-05</v>
@@ -1745,64 +1745,64 @@
         <v>0.0003963243970200002</v>
       </c>
       <c r="S3" t="n">
-        <v>-0.0006823775665430001</v>
+        <v>0.0006823775665430001</v>
       </c>
       <c r="T3" t="n">
-        <v>0.002552003787653</v>
+        <v>0.004104612738061</v>
       </c>
       <c r="U3" t="n">
-        <v>-0.02571633372177488</v>
+        <v>0.175743658039772</v>
       </c>
       <c r="V3" t="n">
-        <v>-0.1529839207315712</v>
+        <v>0.02954220638367767</v>
       </c>
       <c r="W3" t="n">
-        <v>0.1037889785157233</v>
+        <v>0.02697157010161872</v>
       </c>
       <c r="X3" t="n">
-        <v>7240.794740056002</v>
+        <v>6033.995616713335</v>
       </c>
       <c r="Y3" t="n">
-        <v>180.84679</v>
+        <v>150.70566</v>
       </c>
       <c r="Z3" t="n">
-        <v>180.48534</v>
+        <v>150.40445</v>
       </c>
       <c r="AA3" t="n">
-        <v>3234.381354196</v>
+        <v>2695.317795163333</v>
       </c>
       <c r="AB3" t="n">
-        <v>3422.235171518</v>
+        <v>2851.862642931667</v>
       </c>
       <c r="AC3" t="n">
-        <v>7240.794740056</v>
+        <v>6033.995616713333</v>
       </c>
       <c r="AD3" t="n">
-        <v>6558.417173512999</v>
+        <v>5465.347644594167</v>
       </c>
       <c r="AE3" t="n">
-        <v>-187.853817322</v>
+        <v>156.5448477683333</v>
       </c>
       <c r="AF3" t="n">
-        <v>-682.3775665430001</v>
+        <v>568.6479721191668</v>
       </c>
       <c r="AG3" t="n">
-        <v>89.65446512100009</v>
+        <v>74.71205426750008</v>
       </c>
       <c r="AH3" t="n">
-        <v>396.3243970200002</v>
+        <v>330.2703308500002</v>
       </c>
       <c r="AI3" t="n">
-        <v>89.65446512100009</v>
+        <v>74.71205426750008</v>
       </c>
       <c r="AJ3" t="n">
-        <v>396.3243970200002</v>
+        <v>330.2703308500002</v>
       </c>
       <c r="AK3" t="n">
-        <v>-682.3775665430001</v>
+        <v>568.6479721191668</v>
       </c>
       <c r="AL3" t="n">
-        <v>2552.003787653</v>
+        <v>3420.510615050834</v>
       </c>
       <c r="AM3" t="n">
         <v>3.234381354196</v>
@@ -1817,10 +1817,10 @@
         <v>6.558417173513</v>
       </c>
       <c r="AQ3" t="n">
-        <v>-0.187853817322</v>
+        <v>0.187853817322</v>
       </c>
       <c r="AR3" t="n">
-        <v>-0.6823775665430001</v>
+        <v>0.6823775665430001</v>
       </c>
       <c r="AS3" t="n">
         <v>0.08965446512100009</v>
@@ -1835,10 +1835,10 @@
         <v>0.3963243970200002</v>
       </c>
       <c r="AW3" t="n">
-        <v>-0.6823775665430001</v>
+        <v>0.6823775665430001</v>
       </c>
       <c r="AX3" t="n">
-        <v>2.552003787653</v>
+        <v>4.104612738061</v>
       </c>
     </row>
     <row r="4">
@@ -1884,7 +1884,7 @@
         <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>-0.0006823775665430001</v>
+        <v>0.0006823775665430001</v>
       </c>
       <c r="Q4" t="n">
         <v>0.003324035819317</v>
@@ -1893,22 +1893,22 @@
         <v>0.003818559568538</v>
       </c>
       <c r="S4" t="n">
-        <v>-0.0006823775665430001</v>
+        <v>0.0006823775665430001</v>
       </c>
       <c r="T4" t="n">
-        <v>-0.0006823775665430001</v>
+        <v>0.0006823775665430001</v>
       </c>
       <c r="U4" t="n">
-        <v>0.9193915247663157</v>
+        <v>1.233823951224215</v>
       </c>
       <c r="V4" t="n">
-        <v>-1.152983920731571</v>
+        <v>-0.9704577936163223</v>
       </c>
       <c r="W4" t="n">
-        <v>1.103788978515723</v>
+        <v>1.026971570101619</v>
       </c>
       <c r="X4" t="n">
-        <v>7240.794740056002</v>
+        <v>6033.995616713335</v>
       </c>
       <c r="Y4" t="inlineStr"/>
       <c r="Z4" t="inlineStr"/>
@@ -1919,34 +1919,34 @@
         <v>0</v>
       </c>
       <c r="AC4" t="n">
-        <v>7240.794740056</v>
+        <v>6033.995616713333</v>
       </c>
       <c r="AD4" t="n">
-        <v>6558.417173512999</v>
+        <v>5465.347644594167</v>
       </c>
       <c r="AE4" t="n">
         <v>0</v>
       </c>
       <c r="AF4" t="n">
-        <v>-682.3775665430001</v>
+        <v>568.6479721191668</v>
       </c>
       <c r="AG4" t="n">
-        <v>3234.381354196</v>
+        <v>2695.317795163333</v>
       </c>
       <c r="AH4" t="n">
-        <v>3422.235171518</v>
+        <v>2851.862642931667</v>
       </c>
       <c r="AI4" t="n">
-        <v>3324.035819317</v>
+        <v>2770.029849430834</v>
       </c>
       <c r="AJ4" t="n">
-        <v>3818.559568538</v>
+        <v>3182.132973781667</v>
       </c>
       <c r="AK4" t="n">
-        <v>-682.3775665430001</v>
+        <v>568.6479721191668</v>
       </c>
       <c r="AL4" t="n">
-        <v>-682.3775665430001</v>
+        <v>568.6479721191668</v>
       </c>
       <c r="AM4" t="n">
         <v>0</v>
@@ -1964,7 +1964,7 @@
         <v>0</v>
       </c>
       <c r="AR4" t="n">
-        <v>-0.6823775665430001</v>
+        <v>0.6823775665430001</v>
       </c>
       <c r="AS4" t="n">
         <v>3.234381354196</v>
@@ -1979,10 +1979,10 @@
         <v>3.818559568538</v>
       </c>
       <c r="AW4" t="n">
-        <v>-0.6823775665430001</v>
+        <v>0.6823775665430001</v>
       </c>
       <c r="AX4" t="n">
-        <v>-0.6823775665430001</v>
+        <v>0.6823775665430001</v>
       </c>
     </row>
     <row r="5">
@@ -2011,10 +2011,10 @@
         <v>0.003287683004216</v>
       </c>
       <c r="I5" t="n">
-        <v>101.3235504255489</v>
+        <v>98.69373860273339</v>
       </c>
       <c r="J5" t="n">
-        <v>322.0087885378085</v>
+        <v>280.2539932277926</v>
       </c>
       <c r="K5" t="n">
         <v>0.010571991886665</v>
@@ -2029,10 +2029,10 @@
         <v>-0.003331197146609</v>
       </c>
       <c r="O5" t="n">
-        <v>-4.351414239299987e-05</v>
+        <v>4.351414239299987e-05</v>
       </c>
       <c r="P5" t="n">
-        <v>-0.000725891708936</v>
+        <v>0.000725891708936</v>
       </c>
       <c r="Q5" t="n">
         <v>3.635281510100006e-05</v>
@@ -2041,10 +2041,10 @@
         <v>0.0004873624219290003</v>
       </c>
       <c r="S5" t="n">
-        <v>-0.000725891708936</v>
+        <v>0.000725891708936</v>
       </c>
       <c r="T5" t="n">
-        <v>0.00256179129528</v>
+        <v>0.004057088855545</v>
       </c>
       <c r="U5" t="inlineStr">
         <is>
@@ -2062,49 +2062,49 @@
         </is>
       </c>
       <c r="X5" t="n">
-        <v>10571.991886665</v>
+        <v>8809.993238887502</v>
       </c>
       <c r="Y5" t="n">
-        <v>724.6024200000001</v>
+        <v>603.8353499999999</v>
       </c>
       <c r="Z5" t="n">
-        <v>724.12467</v>
+        <v>603.43722</v>
       </c>
       <c r="AA5" t="n">
-        <v>3287.683004216</v>
+        <v>2739.735836846667</v>
       </c>
       <c r="AB5" t="n">
-        <v>3331.197146609</v>
+        <v>2775.997622174167</v>
       </c>
       <c r="AC5" t="n">
-        <v>10571.991886665</v>
+        <v>8809.9932388875</v>
       </c>
       <c r="AD5" t="n">
-        <v>9846.100177729</v>
+        <v>8205.083481440834</v>
       </c>
       <c r="AE5" t="n">
-        <v>-43.51414239299987</v>
+        <v>36.26178532749989</v>
       </c>
       <c r="AF5" t="n">
-        <v>-725.891708936</v>
+        <v>604.9097574466666</v>
       </c>
       <c r="AG5" t="n">
-        <v>-3287.683004216</v>
+        <v>-2739.735836846667</v>
       </c>
       <c r="AH5" t="n">
-        <v>-3331.197146609</v>
+        <v>-2775.997622174167</v>
       </c>
       <c r="AI5" t="n">
-        <v>36.35281510100006</v>
+        <v>30.29401258416672</v>
       </c>
       <c r="AJ5" t="n">
-        <v>487.3624219290003</v>
+        <v>406.1353516075002</v>
       </c>
       <c r="AK5" t="n">
-        <v>-725.891708936</v>
+        <v>604.9097574466666</v>
       </c>
       <c r="AL5" t="n">
-        <v>2561.79129528</v>
+        <v>3380.907379620833</v>
       </c>
       <c r="AM5" t="n">
         <v>3.287683004216</v>
@@ -2119,10 +2119,10 @@
         <v>9.846100177728999</v>
       </c>
       <c r="AQ5" t="n">
-        <v>-0.04351414239299987</v>
+        <v>0.04351414239299987</v>
       </c>
       <c r="AR5" t="n">
-        <v>-0.725891708936</v>
+        <v>0.725891708936</v>
       </c>
       <c r="AS5" t="n">
         <v>-3.287683004216</v>
@@ -2137,10 +2137,10 @@
         <v>0.4873624219290003</v>
       </c>
       <c r="AW5" t="n">
-        <v>-0.725891708936</v>
+        <v>0.725891708936</v>
       </c>
       <c r="AX5" t="n">
-        <v>2.56179129528</v>
+        <v>4.057088855545</v>
       </c>
     </row>
     <row r="6">
@@ -2169,10 +2169,10 @@
         <v>0.003391848714922</v>
       </c>
       <c r="I6" t="n">
-        <v>98.98869478334653</v>
+        <v>101.0216370857974</v>
       </c>
       <c r="J6" t="n">
-        <v>420.9974833211551</v>
+        <v>381.2756303135901</v>
       </c>
       <c r="K6" t="n">
         <v>0.013929538658592</v>
@@ -2187,10 +2187,10 @@
         <v>-2.634962531800024e-05</v>
       </c>
       <c r="O6" t="n">
-        <v>3.430194299499983e-05</v>
+        <v>-3.430194299499983e-05</v>
       </c>
       <c r="P6" t="n">
-        <v>-0.0006915897659410001</v>
+        <v>0.0006915897659410001</v>
       </c>
       <c r="Q6" t="n">
         <v>-6.781289560499988e-05</v>
@@ -2199,10 +2199,10 @@
         <v>0.000461012796611</v>
       </c>
       <c r="S6" t="n">
-        <v>-0.0006915897659410001</v>
+        <v>0.0006915897659410001</v>
       </c>
       <c r="T6" t="n">
-        <v>0.002700258948981</v>
+        <v>0.004049136537868</v>
       </c>
       <c r="U6" t="inlineStr">
         <is>
@@ -2220,49 +2220,49 @@
         </is>
       </c>
       <c r="X6" t="n">
-        <v>13929.538658592</v>
+        <v>11607.94888216</v>
       </c>
       <c r="Y6" t="n">
-        <v>724.62012</v>
+        <v>603.8501</v>
       </c>
       <c r="Z6" t="n">
-        <v>724.1258</v>
+        <v>603.43817</v>
       </c>
       <c r="AA6" t="n">
-        <v>3391.848714922</v>
+        <v>2826.540595768333</v>
       </c>
       <c r="AB6" t="n">
-        <v>3357.546771927</v>
+        <v>2797.9556432725</v>
       </c>
       <c r="AC6" t="n">
-        <v>13929.538658592</v>
+        <v>11607.94888216</v>
       </c>
       <c r="AD6" t="n">
-        <v>13237.948892651</v>
+        <v>11031.62407720917</v>
       </c>
       <c r="AE6" t="n">
-        <v>34.30194299499983</v>
+        <v>-28.58495249583319</v>
       </c>
       <c r="AF6" t="n">
-        <v>-691.5897659410001</v>
+        <v>576.3248049508335</v>
       </c>
       <c r="AG6" t="n">
-        <v>-104.1657107059999</v>
+        <v>-86.80475892166662</v>
       </c>
       <c r="AH6" t="n">
-        <v>-26.34962531800024</v>
+        <v>-21.95802109833353</v>
       </c>
       <c r="AI6" t="n">
-        <v>-67.81289560499988</v>
+        <v>-56.5107463374999</v>
       </c>
       <c r="AJ6" t="n">
-        <v>461.0127966110001</v>
+        <v>384.1773305091667</v>
       </c>
       <c r="AK6" t="n">
-        <v>-691.5897659410001</v>
+        <v>576.3248049508335</v>
       </c>
       <c r="AL6" t="n">
-        <v>2700.258948981</v>
+        <v>3374.280448223334</v>
       </c>
       <c r="AM6" t="n">
         <v>3.391848714922</v>
@@ -2277,10 +2277,10 @@
         <v>13.237948892651</v>
       </c>
       <c r="AQ6" t="n">
-        <v>0.03430194299499983</v>
+        <v>-0.03430194299499983</v>
       </c>
       <c r="AR6" t="n">
-        <v>-0.6915897659410001</v>
+        <v>0.6915897659410001</v>
       </c>
       <c r="AS6" t="n">
         <v>-0.1041657107059999</v>
@@ -2295,10 +2295,10 @@
         <v>0.461012796611</v>
       </c>
       <c r="AW6" t="n">
-        <v>-0.6915897659410001</v>
+        <v>0.6915897659410001</v>
       </c>
       <c r="AX6" t="n">
-        <v>2.700258948981</v>
+        <v>4.049136537868</v>
       </c>
     </row>
     <row r="7">
@@ -2327,10 +2327,10 @@
         <v>0.003435421762151</v>
       </c>
       <c r="I7" t="n">
-        <v>103.8617312606163</v>
+        <v>96.2818535626696</v>
       </c>
       <c r="J7" t="n">
-        <v>524.8592145817713</v>
+        <v>477.5574838762597</v>
       </c>
       <c r="K7" t="n">
         <v>0.017497627176866</v>
@@ -2345,10 +2345,10 @@
         <v>-0.0002105417463470001</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.0001326667561230002</v>
+        <v>0.0001326667561230002</v>
       </c>
       <c r="P7" t="n">
-        <v>-0.0008242565220640003</v>
+        <v>0.0008242565220640003</v>
       </c>
       <c r="Q7" t="n">
         <v>-0.000111385942834</v>
@@ -2357,10 +2357,10 @@
         <v>0.0002504710502639999</v>
       </c>
       <c r="S7" t="n">
-        <v>-0.0008242565220640003</v>
+        <v>0.0008242565220640003</v>
       </c>
       <c r="T7" t="n">
-        <v>0.002611165240087</v>
+        <v>0.004392345040338001</v>
       </c>
       <c r="U7" t="inlineStr">
         <is>
@@ -2378,49 +2378,49 @@
         </is>
       </c>
       <c r="X7" t="n">
-        <v>17497.627176866</v>
+        <v>14581.35598072167</v>
       </c>
       <c r="Y7" t="n">
-        <v>180.84716</v>
+        <v>150.70596</v>
       </c>
       <c r="Z7" t="n">
-        <v>180.45366</v>
+        <v>150.37805</v>
       </c>
       <c r="AA7" t="n">
-        <v>3435.421762151</v>
+        <v>2862.851468459167</v>
       </c>
       <c r="AB7" t="n">
-        <v>3568.088518274</v>
+        <v>2973.407098561667</v>
       </c>
       <c r="AC7" t="n">
-        <v>17497.627176866</v>
+        <v>14581.35598072167</v>
       </c>
       <c r="AD7" t="n">
-        <v>16673.370654802</v>
+        <v>13894.47554566833</v>
       </c>
       <c r="AE7" t="n">
-        <v>-132.6667561230002</v>
+        <v>110.5556301025002</v>
       </c>
       <c r="AF7" t="n">
-        <v>-824.2565220640004</v>
+        <v>686.8804350533336</v>
       </c>
       <c r="AG7" t="n">
-        <v>-43.5730472290001</v>
+        <v>-36.31087269083342</v>
       </c>
       <c r="AH7" t="n">
-        <v>-210.5417463470001</v>
+        <v>-175.4514552891668</v>
       </c>
       <c r="AI7" t="n">
-        <v>-111.385942834</v>
+        <v>-92.82161902833332</v>
       </c>
       <c r="AJ7" t="n">
-        <v>250.4710502639999</v>
+        <v>208.7258752199999</v>
       </c>
       <c r="AK7" t="n">
-        <v>-824.2565220640004</v>
+        <v>686.8804350533336</v>
       </c>
       <c r="AL7" t="n">
-        <v>2611.165240087</v>
+        <v>3660.287533615001</v>
       </c>
       <c r="AM7" t="n">
         <v>3.435421762151</v>
@@ -2435,10 +2435,10 @@
         <v>16.673370654802</v>
       </c>
       <c r="AQ7" t="n">
-        <v>-0.1326667561230002</v>
+        <v>0.1326667561230002</v>
       </c>
       <c r="AR7" t="n">
-        <v>-0.8242565220640004</v>
+        <v>0.8242565220640004</v>
       </c>
       <c r="AS7" t="n">
         <v>-0.0435730472290001</v>
@@ -2453,10 +2453,10 @@
         <v>0.250471050264</v>
       </c>
       <c r="AW7" t="n">
-        <v>-0.8242565220640004</v>
+        <v>0.8242565220640004</v>
       </c>
       <c r="AX7" t="n">
-        <v>2.611165240087</v>
+        <v>4.392345040338001</v>
       </c>
     </row>
     <row r="8">
@@ -2485,10 +2485,10 @@
         <v>0.003485465723957</v>
       </c>
       <c r="I8" t="n">
-        <v>102.4698091671454</v>
+        <v>97.58972014565119</v>
       </c>
       <c r="J8" t="n">
-        <v>627.3290237489167</v>
+        <v>575.1472040219109</v>
       </c>
       <c r="K8" t="n">
         <v>0.021069177252791</v>
@@ -2503,10 +2503,10 @@
         <v>-3.461557650999772e-06</v>
       </c>
       <c r="O8" t="n">
-        <v>-8.608435196800004e-05</v>
+        <v>8.608435196800004e-05</v>
       </c>
       <c r="P8" t="n">
-        <v>-0.0009103408740320004</v>
+        <v>0.0009103408740320004</v>
       </c>
       <c r="Q8" t="n">
         <v>-0.0001614299046399999</v>
@@ -2515,10 +2515,10 @@
         <v>0.0002470094926130002</v>
       </c>
       <c r="S8" t="n">
-        <v>-0.0009103408740320004</v>
+        <v>0.0009103408740320004</v>
       </c>
       <c r="T8" t="n">
-        <v>0.002575124849925</v>
+        <v>0.004481890949957001</v>
       </c>
       <c r="U8" t="inlineStr">
         <is>
@@ -2536,49 +2536,49 @@
         </is>
       </c>
       <c r="X8" t="n">
-        <v>21069.177252791</v>
+        <v>17557.64771065917</v>
       </c>
       <c r="Y8" t="n">
-        <v>180.85294</v>
+        <v>150.71078</v>
       </c>
       <c r="Z8" t="n">
-        <v>180.4316</v>
+        <v>150.35966</v>
       </c>
       <c r="AA8" t="n">
-        <v>3485.465723957</v>
+        <v>2904.554769964167</v>
       </c>
       <c r="AB8" t="n">
-        <v>3571.550075925</v>
+        <v>2976.2917299375</v>
       </c>
       <c r="AC8" t="n">
-        <v>21069.177252791</v>
+        <v>17557.64771065917</v>
       </c>
       <c r="AD8" t="n">
-        <v>20158.836378759</v>
+        <v>16799.0303156325</v>
       </c>
       <c r="AE8" t="n">
-        <v>-86.08435196800005</v>
+        <v>71.73695997333337</v>
       </c>
       <c r="AF8" t="n">
-        <v>-910.3408740320003</v>
+        <v>758.6173950266671</v>
       </c>
       <c r="AG8" t="n">
-        <v>-50.04396180599991</v>
+        <v>-41.70330150499993</v>
       </c>
       <c r="AH8" t="n">
-        <v>-3.461557650999772</v>
+        <v>-2.884631375833143</v>
       </c>
       <c r="AI8" t="n">
-        <v>-161.4299046399999</v>
+        <v>-134.5249205333332</v>
       </c>
       <c r="AJ8" t="n">
-        <v>247.0094926130002</v>
+        <v>205.8412438441668</v>
       </c>
       <c r="AK8" t="n">
-        <v>-910.3408740320003</v>
+        <v>758.6173950266671</v>
       </c>
       <c r="AL8" t="n">
-        <v>2575.124849925</v>
+        <v>3734.909124964167</v>
       </c>
       <c r="AM8" t="n">
         <v>3.485465723957</v>
@@ -2593,10 +2593,10 @@
         <v>20.158836378759</v>
       </c>
       <c r="AQ8" t="n">
-        <v>-0.08608435196800004</v>
+        <v>0.08608435196800004</v>
       </c>
       <c r="AR8" t="n">
-        <v>-0.9103408740320004</v>
+        <v>0.9103408740320004</v>
       </c>
       <c r="AS8" t="n">
         <v>-0.05004396180599991</v>
@@ -2611,10 +2611,10 @@
         <v>0.2470094926130001</v>
       </c>
       <c r="AW8" t="n">
-        <v>-0.9103408740320004</v>
+        <v>0.9103408740320004</v>
       </c>
       <c r="AX8" t="n">
-        <v>2.575124849924999</v>
+        <v>4.481890949957001</v>
       </c>
     </row>
     <row r="9">
@@ -2643,10 +2643,10 @@
         <v>0.003494661625918</v>
       </c>
       <c r="I9" t="n">
-        <v>103.3571586258278</v>
+        <v>96.75188572280578</v>
       </c>
       <c r="J9" t="n">
-        <v>730.6861823747445</v>
+        <v>671.8990897447167</v>
       </c>
       <c r="K9" t="n">
         <v>0.024681160212927</v>
@@ -2661,10 +2661,10 @@
         <v>-4.043288421099996e-05</v>
       </c>
       <c r="O9" t="n">
-        <v>-0.0001173213342179997</v>
+        <v>0.0001173213342179997</v>
       </c>
       <c r="P9" t="n">
-        <v>-0.00102766220825</v>
+        <v>0.00102766220825</v>
       </c>
       <c r="Q9" t="n">
         <v>-0.0001706258066010002</v>
@@ -2673,10 +2673,10 @@
         <v>0.0002065766084020002</v>
       </c>
       <c r="S9" t="n">
-        <v>-0.00102766220825</v>
+        <v>0.00102766220825</v>
       </c>
       <c r="T9" t="n">
-        <v>0.002466999417668</v>
+        <v>0.004639645168386</v>
       </c>
       <c r="U9" t="inlineStr">
         <is>
@@ -2694,49 +2694,49 @@
         </is>
       </c>
       <c r="X9" t="n">
-        <v>24681.160212927</v>
+        <v>20567.6335107725</v>
       </c>
       <c r="Y9" t="n">
-        <v>180.84635</v>
+        <v>150.70529</v>
       </c>
       <c r="Z9" t="n">
-        <v>180.53224</v>
+        <v>150.44354</v>
       </c>
       <c r="AA9" t="n">
-        <v>3494.661625918</v>
+        <v>2912.218021598334</v>
       </c>
       <c r="AB9" t="n">
-        <v>3611.982960136</v>
+        <v>3009.985800113333</v>
       </c>
       <c r="AC9" t="n">
-        <v>24681.160212927</v>
+        <v>20567.6335107725</v>
       </c>
       <c r="AD9" t="n">
-        <v>23653.498004677</v>
+        <v>19711.24833723083</v>
       </c>
       <c r="AE9" t="n">
-        <v>-117.3213342179997</v>
+        <v>97.76777851499978</v>
       </c>
       <c r="AF9" t="n">
-        <v>-1027.66220825</v>
+        <v>856.3851735416667</v>
       </c>
       <c r="AG9" t="n">
-        <v>-9.195901961000283</v>
+        <v>-7.663251634166902</v>
       </c>
       <c r="AH9" t="n">
-        <v>-40.43288421099996</v>
+        <v>-33.6940701758333</v>
       </c>
       <c r="AI9" t="n">
-        <v>-170.6258066010002</v>
+        <v>-142.1881721675001</v>
       </c>
       <c r="AJ9" t="n">
-        <v>206.5766084020002</v>
+        <v>172.1471736683335</v>
       </c>
       <c r="AK9" t="n">
-        <v>-1027.66220825</v>
+        <v>856.3851735416667</v>
       </c>
       <c r="AL9" t="n">
-        <v>2466.999417668</v>
+        <v>3866.370973655</v>
       </c>
       <c r="AM9" t="n">
         <v>3.494661625918</v>
@@ -2751,10 +2751,10 @@
         <v>23.653498004677</v>
       </c>
       <c r="AQ9" t="n">
-        <v>-0.1173213342179997</v>
+        <v>0.1173213342179997</v>
       </c>
       <c r="AR9" t="n">
-        <v>-1.02766220825</v>
+        <v>1.02766220825</v>
       </c>
       <c r="AS9" t="n">
         <v>-0.009195901961000282</v>
@@ -2769,10 +2769,10 @@
         <v>0.2065766084020002</v>
       </c>
       <c r="AW9" t="n">
-        <v>-1.02766220825</v>
+        <v>1.02766220825</v>
       </c>
       <c r="AX9" t="n">
-        <v>2.466999417668</v>
+        <v>4.639645168386</v>
       </c>
     </row>
     <row r="10">
@@ -2801,10 +2801,10 @@
         <v>0.003404127582165</v>
       </c>
       <c r="I10" t="n">
-        <v>104.0556867482679</v>
+        <v>96.1023881778999</v>
       </c>
       <c r="J10" t="n">
-        <v>834.7418691230124</v>
+        <v>768.0014779226166</v>
       </c>
       <c r="K10" t="n">
         <v>0.028223348546336</v>
@@ -2819,10 +2819,10 @@
         <v>6.979462672699992e-05</v>
       </c>
       <c r="O10" t="n">
-        <v>-0.0001380607512439999</v>
+        <v>0.0001380607512439999</v>
       </c>
       <c r="P10" t="n">
-        <v>-0.001165722959494</v>
+        <v>0.001165722959494</v>
       </c>
       <c r="Q10" t="n">
         <v>-8.009176284800006e-05</v>
@@ -2831,10 +2831,10 @@
         <v>0.0002763712351290001</v>
       </c>
       <c r="S10" t="n">
-        <v>-0.001165722959494</v>
+        <v>0.001165722959494</v>
       </c>
       <c r="T10" t="n">
-        <v>0.002238404622671</v>
+        <v>0.004707911292903</v>
       </c>
       <c r="U10" t="inlineStr">
         <is>
@@ -2852,49 +2852,49 @@
         </is>
       </c>
       <c r="X10" t="n">
-        <v>28223.348546336</v>
+        <v>23519.45712194667</v>
       </c>
       <c r="Y10" t="n">
-        <v>363.04386</v>
+        <v>302.53655</v>
       </c>
       <c r="Z10" t="n">
-        <v>362.66427</v>
+        <v>302.22022</v>
       </c>
       <c r="AA10" t="n">
-        <v>3404.127582165</v>
+        <v>2836.7729851375</v>
       </c>
       <c r="AB10" t="n">
-        <v>3542.188333409</v>
+        <v>2951.823611174167</v>
       </c>
       <c r="AC10" t="n">
-        <v>28223.348546336</v>
+        <v>23519.45712194666</v>
       </c>
       <c r="AD10" t="n">
-        <v>27057.625586842</v>
+        <v>22548.02132236833</v>
       </c>
       <c r="AE10" t="n">
-        <v>-138.0607512439999</v>
+        <v>115.0506260366666</v>
       </c>
       <c r="AF10" t="n">
-        <v>-1165.722959494</v>
+        <v>971.4357995783333</v>
       </c>
       <c r="AG10" t="n">
-        <v>90.53404375300011</v>
+        <v>75.44503646083342</v>
       </c>
       <c r="AH10" t="n">
-        <v>69.79462672699992</v>
+        <v>58.1621889391666</v>
       </c>
       <c r="AI10" t="n">
-        <v>-80.09176284800006</v>
+        <v>-66.74313570666672</v>
       </c>
       <c r="AJ10" t="n">
-        <v>276.3712351290001</v>
+        <v>230.3093626075001</v>
       </c>
       <c r="AK10" t="n">
-        <v>-1165.722959494</v>
+        <v>971.4357995783333</v>
       </c>
       <c r="AL10" t="n">
-        <v>2238.404622671</v>
+        <v>3923.2594107525</v>
       </c>
       <c r="AM10" t="n">
         <v>3.404127582165</v>
@@ -2909,10 +2909,10 @@
         <v>27.057625586842</v>
       </c>
       <c r="AQ10" t="n">
-        <v>-0.1380607512439999</v>
+        <v>0.1380607512439999</v>
       </c>
       <c r="AR10" t="n">
-        <v>-1.165722959494</v>
+        <v>1.165722959494</v>
       </c>
       <c r="AS10" t="n">
         <v>0.09053404375300012</v>
@@ -2927,10 +2927,10 @@
         <v>0.2763712351290001</v>
       </c>
       <c r="AW10" t="n">
-        <v>-1.165722959494</v>
+        <v>1.165722959494</v>
       </c>
       <c r="AX10" t="n">
-        <v>2.238404622671</v>
+        <v>4.707911292903</v>
       </c>
     </row>
     <row r="11">
@@ -2959,10 +2959,10 @@
         <v>0.003407980409796</v>
       </c>
       <c r="I11" t="n">
-        <v>101.8270968844192</v>
+        <v>98.20568695335281</v>
       </c>
       <c r="J11" t="n">
-        <v>936.5689660074316</v>
+        <v>866.2071648759694</v>
       </c>
       <c r="K11" t="n">
         <v>0.03169359606002099</v>
@@ -2977,10 +2977,10 @@
         <v>7.194081972399999e-05</v>
       </c>
       <c r="O11" t="n">
-        <v>-6.22671038889998e-05</v>
+        <v>6.22671038889998e-05</v>
       </c>
       <c r="P11" t="n">
-        <v>-0.001227990063383</v>
+        <v>0.001227990063383</v>
       </c>
       <c r="Q11" t="n">
         <v>-8.394459047900019e-05</v>
@@ -2989,10 +2989,10 @@
         <v>0.0003483120548530001</v>
       </c>
       <c r="S11" t="n">
-        <v>-0.001227990063383</v>
+        <v>0.001227990063383</v>
       </c>
       <c r="T11" t="n">
-        <v>0.002179990346413</v>
+        <v>0.004698237577068</v>
       </c>
       <c r="U11" t="inlineStr">
         <is>
@@ -3010,49 +3010,49 @@
         </is>
       </c>
       <c r="X11" t="n">
-        <v>31693.596060021</v>
+        <v>26411.3300500175</v>
       </c>
       <c r="Y11" t="n">
-        <v>363.09642</v>
+        <v>302.58035</v>
       </c>
       <c r="Z11" t="n">
-        <v>362.66394</v>
+        <v>302.21995</v>
       </c>
       <c r="AA11" t="n">
-        <v>3407.980409796</v>
+        <v>2839.98367483</v>
       </c>
       <c r="AB11" t="n">
-        <v>3470.247513685</v>
+        <v>2891.872928070833</v>
       </c>
       <c r="AC11" t="n">
-        <v>31693.59606002099</v>
+        <v>26411.3300500175</v>
       </c>
       <c r="AD11" t="n">
-        <v>30465.605996638</v>
+        <v>25388.00499719834</v>
       </c>
       <c r="AE11" t="n">
-        <v>-62.2671038889998</v>
+        <v>51.88925324083317</v>
       </c>
       <c r="AF11" t="n">
-        <v>-1227.990063383</v>
+        <v>1023.325052819167</v>
       </c>
       <c r="AG11" t="n">
-        <v>-3.852827631000127</v>
+        <v>-3.210689692500106</v>
       </c>
       <c r="AH11" t="n">
-        <v>71.94081972399999</v>
+        <v>59.95068310333333</v>
       </c>
       <c r="AI11" t="n">
-        <v>-83.94459047900018</v>
+        <v>-69.95382539916683</v>
       </c>
       <c r="AJ11" t="n">
-        <v>348.3120548530001</v>
+        <v>290.2600457108334</v>
       </c>
       <c r="AK11" t="n">
-        <v>-1227.990063383</v>
+        <v>1023.325052819167</v>
       </c>
       <c r="AL11" t="n">
-        <v>2179.990346413</v>
+        <v>3915.197980890001</v>
       </c>
       <c r="AM11" t="n">
         <v>3.407980409796</v>
@@ -3067,10 +3067,10 @@
         <v>30.465605996638</v>
       </c>
       <c r="AQ11" t="n">
-        <v>-0.06226710388899979</v>
+        <v>0.06226710388899979</v>
       </c>
       <c r="AR11" t="n">
-        <v>-1.227990063383</v>
+        <v>1.227990063383</v>
       </c>
       <c r="AS11" t="n">
         <v>-0.003852827631000127</v>
@@ -3085,10 +3085,10 @@
         <v>0.3483120548530001</v>
       </c>
       <c r="AW11" t="n">
-        <v>-1.227990063383</v>
+        <v>1.227990063383</v>
       </c>
       <c r="AX11" t="n">
-        <v>2.179990346413001</v>
+        <v>4.698237577068</v>
       </c>
     </row>
     <row r="12">
@@ -3117,10 +3117,10 @@
         <v>0.003424037760495</v>
       </c>
       <c r="I12" t="n">
-        <v>101.2222184657493</v>
+        <v>98.7925393413869</v>
       </c>
       <c r="J12" t="n">
-        <v>1037.791184473181</v>
+        <v>964.9997042173563</v>
       </c>
       <c r="K12" t="n">
         <v>0.03515948304229899</v>
@@ -3135,10 +3135,10 @@
         <v>4.360531407000129e-06</v>
       </c>
       <c r="O12" t="n">
-        <v>-4.1849221783e-05</v>
+        <v>4.1849221783e-05</v>
       </c>
       <c r="P12" t="n">
-        <v>-0.001269839285166</v>
+        <v>0.001269839285166</v>
       </c>
       <c r="Q12" t="n">
         <v>-0.0001000019411779999</v>
@@ -3147,10 +3147,10 @@
         <v>0.0003526725862600002</v>
       </c>
       <c r="S12" t="n">
-        <v>-0.001269839285166</v>
+        <v>0.001269839285166</v>
       </c>
       <c r="T12" t="n">
-        <v>0.002154198475329</v>
+        <v>0.004735726267444</v>
       </c>
       <c r="U12" t="inlineStr">
         <is>
@@ -3168,49 +3168,49 @@
         </is>
       </c>
       <c r="X12" t="n">
-        <v>35159.483042299</v>
+        <v>29299.56920191583</v>
       </c>
       <c r="Y12" t="n">
-        <v>363.04371</v>
+        <v>302.53642</v>
       </c>
       <c r="Z12" t="n">
-        <v>362.68092</v>
+        <v>302.2341</v>
       </c>
       <c r="AA12" t="n">
-        <v>3424.037760495</v>
+        <v>2853.3648004125</v>
       </c>
       <c r="AB12" t="n">
-        <v>3465.886982278</v>
+        <v>2888.239151898333</v>
       </c>
       <c r="AC12" t="n">
-        <v>35159.48304229899</v>
+        <v>29299.56920191583</v>
       </c>
       <c r="AD12" t="n">
-        <v>33889.643757133</v>
+        <v>28241.36979761083</v>
       </c>
       <c r="AE12" t="n">
-        <v>-41.849221783</v>
+        <v>34.87435148583334</v>
       </c>
       <c r="AF12" t="n">
-        <v>-1269.839285166</v>
+        <v>1058.199404305</v>
       </c>
       <c r="AG12" t="n">
-        <v>-16.05735069899967</v>
+        <v>-13.38112558249972</v>
       </c>
       <c r="AH12" t="n">
-        <v>4.360531407000129</v>
+        <v>3.633776172500108</v>
       </c>
       <c r="AI12" t="n">
-        <v>-100.0019411779999</v>
+        <v>-83.33495098166655</v>
       </c>
       <c r="AJ12" t="n">
-        <v>352.6725862600002</v>
+        <v>293.8938218833335</v>
       </c>
       <c r="AK12" t="n">
-        <v>-1269.839285166</v>
+        <v>1058.199404305</v>
       </c>
       <c r="AL12" t="n">
-        <v>2154.198475329</v>
+        <v>3946.438556203334</v>
       </c>
       <c r="AM12" t="n">
         <v>3.424037760495</v>
@@ -3225,10 +3225,10 @@
         <v>33.889643757133</v>
       </c>
       <c r="AQ12" t="n">
-        <v>-0.041849221783</v>
+        <v>0.041849221783</v>
       </c>
       <c r="AR12" t="n">
-        <v>-1.269839285166</v>
+        <v>1.269839285166</v>
       </c>
       <c r="AS12" t="n">
         <v>-0.01605735069899967</v>
@@ -3243,10 +3243,10 @@
         <v>0.3526725862600003</v>
       </c>
       <c r="AW12" t="n">
-        <v>-1.269839285166</v>
+        <v>1.269839285166</v>
       </c>
       <c r="AX12" t="n">
-        <v>2.154198475329</v>
+        <v>4.735726267444</v>
       </c>
     </row>
     <row r="13">
@@ -3275,10 +3275,10 @@
         <v>0.00329784552386</v>
       </c>
       <c r="I13" t="n">
-        <v>103.10630901341</v>
+        <v>96.98727551870181</v>
       </c>
       <c r="J13" t="n">
-        <v>1140.897493486591</v>
+        <v>1061.986979736058</v>
       </c>
       <c r="K13" t="n">
         <v>0.03855976983891499</v>
@@ -3293,10 +3293,10 @@
         <v>6.560018566199996e-05</v>
       </c>
       <c r="O13" t="n">
-        <v>-0.0001024412727560001</v>
+        <v>0.0001024412727560001</v>
       </c>
       <c r="P13" t="n">
-        <v>-0.001372280557922</v>
+        <v>0.001372280557922</v>
       </c>
       <c r="Q13" t="n">
         <v>2.619029545700017e-05</v>
@@ -3305,10 +3305,10 @@
         <v>0.0004182727719220002</v>
       </c>
       <c r="S13" t="n">
-        <v>-0.001372280557922</v>
+        <v>0.001372280557922</v>
       </c>
       <c r="T13" t="n">
-        <v>0.001925564965938</v>
+        <v>0.004772567354538</v>
       </c>
       <c r="U13" t="inlineStr">
         <is>
@@ -3326,49 +3326,49 @@
         </is>
       </c>
       <c r="X13" t="n">
-        <v>38559.769838915</v>
+        <v>32133.14153242916</v>
       </c>
       <c r="Y13" t="n">
-        <v>724.67096</v>
+        <v>603.89246</v>
       </c>
       <c r="Z13" t="n">
-        <v>724.17243</v>
+        <v>603.47702</v>
       </c>
       <c r="AA13" t="n">
-        <v>3297.84552386</v>
+        <v>2748.204603216667</v>
       </c>
       <c r="AB13" t="n">
-        <v>3400.286796616</v>
+        <v>2833.572330513333</v>
       </c>
       <c r="AC13" t="n">
-        <v>38559.76983891499</v>
+        <v>32133.14153242916</v>
       </c>
       <c r="AD13" t="n">
-        <v>37187.489280993</v>
+        <v>30989.5744008275</v>
       </c>
       <c r="AE13" t="n">
-        <v>-102.4412727560001</v>
+        <v>85.36772729666673</v>
       </c>
       <c r="AF13" t="n">
-        <v>-1372.280557922</v>
+        <v>1143.567131601667</v>
       </c>
       <c r="AG13" t="n">
-        <v>126.192236635</v>
+        <v>105.1601971958334</v>
       </c>
       <c r="AH13" t="n">
-        <v>65.60018566199996</v>
+        <v>54.66682138499996</v>
       </c>
       <c r="AI13" t="n">
-        <v>26.19029545700016</v>
+        <v>21.82524621416681</v>
       </c>
       <c r="AJ13" t="n">
-        <v>418.2727719220002</v>
+        <v>348.5606432683335</v>
       </c>
       <c r="AK13" t="n">
-        <v>-1372.280557922</v>
+        <v>1143.567131601667</v>
       </c>
       <c r="AL13" t="n">
-        <v>1925.564965938</v>
+        <v>3977.139462115</v>
       </c>
       <c r="AM13" t="n">
         <v>3.29784552386</v>
@@ -3383,10 +3383,10 @@
         <v>37.187489280993</v>
       </c>
       <c r="AQ13" t="n">
-        <v>-0.1024412727560001</v>
+        <v>0.1024412727560001</v>
       </c>
       <c r="AR13" t="n">
-        <v>-1.372280557922</v>
+        <v>1.372280557922</v>
       </c>
       <c r="AS13" t="n">
         <v>0.126192236635</v>
@@ -3401,10 +3401,10 @@
         <v>0.4182727719220002</v>
       </c>
       <c r="AW13" t="n">
-        <v>-1.372280557922</v>
+        <v>1.372280557922</v>
       </c>
       <c r="AX13" t="n">
-        <v>1.925564965938</v>
+        <v>4.772567354537999</v>
       </c>
     </row>
     <row r="14">
@@ -3433,10 +3433,10 @@
         <v>0.003359875445448</v>
       </c>
       <c r="I14" t="n">
-        <v>99.34922406565327</v>
+        <v>100.6550387690161</v>
       </c>
       <c r="J14" t="n">
-        <v>1240.246717552244</v>
+        <v>1162.642018505074</v>
       </c>
       <c r="K14" t="n">
         <v>0.04189778002353998</v>
@@ -3451,10 +3451,10 @@
         <v>6.227661199099998e-05</v>
       </c>
       <c r="O14" t="n">
-        <v>2.186526082300017e-05</v>
+        <v>-2.186526082300017e-05</v>
       </c>
       <c r="P14" t="n">
-        <v>-0.001350415297099</v>
+        <v>0.001350415297099</v>
       </c>
       <c r="Q14" t="n">
         <v>-3.58396261310001e-05</v>
@@ -3463,10 +3463,10 @@
         <v>0.0004805493839130002</v>
       </c>
       <c r="S14" t="n">
-        <v>-0.001350415297099</v>
+        <v>0.001350415297099</v>
       </c>
       <c r="T14" t="n">
-        <v>0.002009460148349</v>
+        <v>0.004688425481724</v>
       </c>
       <c r="U14" t="inlineStr">
         <is>
@@ -3484,49 +3484,49 @@
         </is>
       </c>
       <c r="X14" t="n">
-        <v>41897.78002354</v>
+        <v>34914.81668628333</v>
       </c>
       <c r="Y14" t="n">
-        <v>724.70708</v>
+        <v>603.92257</v>
       </c>
       <c r="Z14" t="n">
-        <v>724.1222299999999</v>
+        <v>603.43519</v>
       </c>
       <c r="AA14" t="n">
-        <v>3359.875445448</v>
+        <v>2799.89620454</v>
       </c>
       <c r="AB14" t="n">
-        <v>3338.010184625</v>
+        <v>2781.675153854167</v>
       </c>
       <c r="AC14" t="n">
-        <v>41897.78002353998</v>
+        <v>34914.81668628332</v>
       </c>
       <c r="AD14" t="n">
-        <v>40547.364726441</v>
+        <v>33789.4706053675</v>
       </c>
       <c r="AE14" t="n">
-        <v>21.86526082300017</v>
+        <v>-18.22105068583348</v>
       </c>
       <c r="AF14" t="n">
-        <v>-1350.415297099</v>
+        <v>1125.346080915833</v>
       </c>
       <c r="AG14" t="n">
-        <v>-62.02992158800026</v>
+        <v>-51.69160132333355</v>
       </c>
       <c r="AH14" t="n">
-        <v>62.27661199099997</v>
+        <v>51.89717665916665</v>
       </c>
       <c r="AI14" t="n">
-        <v>-35.8396261310001</v>
+        <v>-29.86635510916675</v>
       </c>
       <c r="AJ14" t="n">
-        <v>480.5493839130002</v>
+        <v>400.4578199275002</v>
       </c>
       <c r="AK14" t="n">
-        <v>-1350.415297099</v>
+        <v>1125.346080915833</v>
       </c>
       <c r="AL14" t="n">
-        <v>2009.460148349001</v>
+        <v>3907.02123477</v>
       </c>
       <c r="AM14" t="n">
         <v>3.359875445448</v>
@@ -3541,10 +3541,10 @@
         <v>40.547364726441</v>
       </c>
       <c r="AQ14" t="n">
-        <v>0.02186526082300017</v>
+        <v>-0.02186526082300017</v>
       </c>
       <c r="AR14" t="n">
-        <v>-1.350415297099</v>
+        <v>1.350415297099</v>
       </c>
       <c r="AS14" t="n">
         <v>-0.06202992158800026</v>
@@ -3559,10 +3559,10 @@
         <v>0.4805493839130002</v>
       </c>
       <c r="AW14" t="n">
-        <v>-1.350415297099</v>
+        <v>1.350415297099</v>
       </c>
       <c r="AX14" t="n">
-        <v>2.009460148349</v>
+        <v>4.688425481724</v>
       </c>
     </row>
     <row r="15">
@@ -3591,10 +3591,10 @@
         <v>0.003305987401204</v>
       </c>
       <c r="I15" t="n">
-        <v>101.9872638099308</v>
+        <v>98.05145884329789</v>
       </c>
       <c r="J15" t="n">
-        <v>1342.233981362175</v>
+        <v>1260.693477348372</v>
       </c>
       <c r="K15" t="n">
         <v>0.04526946611592898</v>
@@ -3609,10 +3609,10 @@
         <v>-3.367590776400019e-05</v>
       </c>
       <c r="O15" t="n">
-        <v>-6.569869118500018e-05</v>
+        <v>6.569869118500018e-05</v>
       </c>
       <c r="P15" t="n">
-        <v>-0.001416113988284</v>
+        <v>0.001416113988284</v>
       </c>
       <c r="Q15" t="n">
         <v>1.804841811300006e-05</v>
@@ -3621,10 +3621,10 @@
         <v>0.000446873476149</v>
       </c>
       <c r="S15" t="n">
-        <v>-0.001416113988284</v>
+        <v>0.001416113988284</v>
       </c>
       <c r="T15" t="n">
-        <v>0.00188987341292</v>
+        <v>0.004787800080673</v>
       </c>
       <c r="U15" t="inlineStr">
         <is>
@@ -3642,49 +3642,49 @@
         </is>
       </c>
       <c r="X15" t="n">
-        <v>45269.466115929</v>
+        <v>37724.5550966075</v>
       </c>
       <c r="Y15" t="n">
-        <v>724.6967</v>
+        <v>603.91391</v>
       </c>
       <c r="Z15" t="n">
-        <v>724.05727</v>
+        <v>603.38106</v>
       </c>
       <c r="AA15" t="n">
-        <v>3305.987401204</v>
+        <v>2754.989501003333</v>
       </c>
       <c r="AB15" t="n">
-        <v>3371.686092389</v>
+        <v>2809.738410324167</v>
       </c>
       <c r="AC15" t="n">
-        <v>45269.46611592898</v>
+        <v>37724.55509660749</v>
       </c>
       <c r="AD15" t="n">
-        <v>43853.352127645</v>
+        <v>36544.46010637083</v>
       </c>
       <c r="AE15" t="n">
-        <v>-65.69869118500017</v>
+        <v>54.74890932083348</v>
       </c>
       <c r="AF15" t="n">
-        <v>-1416.113988284</v>
+        <v>1180.094990236667</v>
       </c>
       <c r="AG15" t="n">
-        <v>53.88804424400016</v>
+        <v>44.9067035366668</v>
       </c>
       <c r="AH15" t="n">
-        <v>-33.67590776400019</v>
+        <v>-28.06325647000016</v>
       </c>
       <c r="AI15" t="n">
-        <v>18.04841811300006</v>
+        <v>15.04034842750005</v>
       </c>
       <c r="AJ15" t="n">
-        <v>446.873476149</v>
+        <v>372.3945634575</v>
       </c>
       <c r="AK15" t="n">
-        <v>-1416.113988284</v>
+        <v>1180.094990236667</v>
       </c>
       <c r="AL15" t="n">
-        <v>1889.87341292</v>
+        <v>3989.833400560833</v>
       </c>
       <c r="AM15" t="n">
         <v>3.305987401204</v>
@@ -3699,10 +3699,10 @@
         <v>43.853352127645</v>
       </c>
       <c r="AQ15" t="n">
-        <v>-0.06569869118500019</v>
+        <v>0.06569869118500019</v>
       </c>
       <c r="AR15" t="n">
-        <v>-1.416113988284</v>
+        <v>1.416113988284</v>
       </c>
       <c r="AS15" t="n">
         <v>0.05388804424400016</v>
@@ -3717,10 +3717,10 @@
         <v>0.446873476149</v>
       </c>
       <c r="AW15" t="n">
-        <v>-1.416113988284</v>
+        <v>1.416113988284</v>
       </c>
       <c r="AX15" t="n">
-        <v>1.88987341292</v>
+        <v>4.787800080673</v>
       </c>
     </row>
     <row r="16">
@@ -3749,10 +3749,10 @@
         <v>0.003076328468309</v>
       </c>
       <c r="I16" t="n">
-        <v>104.253763588871</v>
+        <v>95.91979853538348</v>
       </c>
       <c r="J16" t="n">
-        <v>1446.487744951046</v>
+        <v>1356.613275883756</v>
       </c>
       <c r="K16" t="n">
         <v>0.04847665432449699</v>
@@ -3767,10 +3767,10 @@
         <v>0.0001644978838210003</v>
       </c>
       <c r="O16" t="n">
-        <v>-0.000130859740259</v>
+        <v>0.000130859740259</v>
       </c>
       <c r="P16" t="n">
-        <v>-0.001546973728543</v>
+        <v>0.001546973728543</v>
       </c>
       <c r="Q16" t="n">
         <v>0.0002477073510080002</v>
@@ -3779,10 +3779,10 @@
         <v>0.0006113713599700003</v>
       </c>
       <c r="S16" t="n">
-        <v>-0.001546973728543</v>
+        <v>0.001546973728543</v>
       </c>
       <c r="T16" t="n">
-        <v>0.001529354739766</v>
+        <v>0.004754161937111</v>
       </c>
       <c r="U16" t="inlineStr">
         <is>
@@ -3800,49 +3800,49 @@
         </is>
       </c>
       <c r="X16" t="n">
-        <v>48476.654324497</v>
+        <v>40397.21193708083</v>
       </c>
       <c r="Y16" t="n">
-        <v>1811.74501</v>
+        <v>1509.78751</v>
       </c>
       <c r="Z16" t="n">
-        <v>1810.94712</v>
+        <v>1509.1226</v>
       </c>
       <c r="AA16" t="n">
-        <v>3076.328468309</v>
+        <v>2563.607056924166</v>
       </c>
       <c r="AB16" t="n">
-        <v>3207.188208568</v>
+        <v>2672.656840473333</v>
       </c>
       <c r="AC16" t="n">
-        <v>48476.65432449699</v>
+        <v>40397.21193708082</v>
       </c>
       <c r="AD16" t="n">
-        <v>46929.68059595399</v>
+        <v>39108.067163295</v>
       </c>
       <c r="AE16" t="n">
-        <v>-130.859740259</v>
+        <v>109.0497835491667</v>
       </c>
       <c r="AF16" t="n">
-        <v>-1546.973728543</v>
+        <v>1289.144773785833</v>
       </c>
       <c r="AG16" t="n">
-        <v>229.6589328950002</v>
+        <v>191.3824440791668</v>
       </c>
       <c r="AH16" t="n">
-        <v>164.4978838210003</v>
+        <v>137.0815698508336</v>
       </c>
       <c r="AI16" t="n">
-        <v>247.7073510080002</v>
+        <v>206.4227925066669</v>
       </c>
       <c r="AJ16" t="n">
-        <v>611.3713599700003</v>
+        <v>509.4761333083336</v>
       </c>
       <c r="AK16" t="n">
-        <v>-1546.973728543</v>
+        <v>1289.144773785833</v>
       </c>
       <c r="AL16" t="n">
-        <v>1529.354739766</v>
+        <v>3961.801614259166</v>
       </c>
       <c r="AM16" t="n">
         <v>3.076328468309</v>
@@ -3857,10 +3857,10 @@
         <v>46.929680595954</v>
       </c>
       <c r="AQ16" t="n">
-        <v>-0.130859740259</v>
+        <v>0.130859740259</v>
       </c>
       <c r="AR16" t="n">
-        <v>-1.546973728543</v>
+        <v>1.546973728543</v>
       </c>
       <c r="AS16" t="n">
         <v>0.2296589328950002</v>
@@ -3875,10 +3875,10 @@
         <v>0.6113713599700002</v>
       </c>
       <c r="AW16" t="n">
-        <v>-1.546973728543</v>
+        <v>1.546973728543</v>
       </c>
       <c r="AX16" t="n">
-        <v>1.529354739766</v>
+        <v>4.754161937110999</v>
       </c>
     </row>
     <row r="17">
@@ -3907,10 +3907,10 @@
         <v>0.002769126357556</v>
       </c>
       <c r="I17" t="n">
-        <v>105.823357681638</v>
+        <v>94.49709609559247</v>
       </c>
       <c r="J17" t="n">
-        <v>1552.311102632684</v>
+        <v>1451.110371979348</v>
       </c>
       <c r="K17" t="n">
         <v>0.05140703681450998</v>
@@ -3925,10 +3925,10 @@
         <v>0.000276805718555</v>
       </c>
       <c r="O17" t="n">
-        <v>-0.000161256132457</v>
+        <v>0.000161256132457</v>
       </c>
       <c r="P17" t="n">
-        <v>-0.001708229861</v>
+        <v>0.001708229861</v>
       </c>
       <c r="Q17" t="n">
         <v>0.0005549094617610002</v>
@@ -3937,10 +3937,10 @@
         <v>0.0008881770785250003</v>
       </c>
       <c r="S17" t="n">
-        <v>-0.001708229861</v>
+        <v>0.001708229861</v>
       </c>
       <c r="T17" t="n">
-        <v>0.001060896496556</v>
+        <v>0.004638612351013</v>
       </c>
       <c r="U17" t="inlineStr">
         <is>
@@ -3958,49 +3958,49 @@
         </is>
       </c>
       <c r="X17" t="n">
-        <v>51407.03681451</v>
+        <v>42839.197345425</v>
       </c>
       <c r="Y17" t="n">
-        <v>3622.37158</v>
+        <v>3018.64298</v>
       </c>
       <c r="Z17" t="n">
-        <v>3621.68782</v>
+        <v>3018.07319</v>
       </c>
       <c r="AA17" t="n">
-        <v>2769.126357556</v>
+        <v>2307.605297963333</v>
       </c>
       <c r="AB17" t="n">
-        <v>2930.382490013</v>
+        <v>2441.985408344166</v>
       </c>
       <c r="AC17" t="n">
-        <v>51407.03681450999</v>
+        <v>42839.19734542499</v>
       </c>
       <c r="AD17" t="n">
-        <v>49698.80695351</v>
+        <v>41415.67246125833</v>
       </c>
       <c r="AE17" t="n">
-        <v>-161.256132457</v>
+        <v>134.3801103808334</v>
       </c>
       <c r="AF17" t="n">
-        <v>-1708.229861</v>
+        <v>1423.524884166667</v>
       </c>
       <c r="AG17" t="n">
-        <v>307.202110753</v>
+        <v>256.0017589608333</v>
       </c>
       <c r="AH17" t="n">
-        <v>276.805718555</v>
+        <v>230.6714321291667</v>
       </c>
       <c r="AI17" t="n">
-        <v>554.9094617610002</v>
+        <v>462.4245514675002</v>
       </c>
       <c r="AJ17" t="n">
-        <v>888.1770785250003</v>
+        <v>740.1475654375002</v>
       </c>
       <c r="AK17" t="n">
-        <v>-1708.229861</v>
+        <v>1423.524884166667</v>
       </c>
       <c r="AL17" t="n">
-        <v>1060.896496556</v>
+        <v>3865.510292510834</v>
       </c>
       <c r="AM17" t="n">
         <v>2.769126357556</v>
@@ -4015,10 +4015,10 @@
         <v>49.69880695351</v>
       </c>
       <c r="AQ17" t="n">
-        <v>-0.161256132457</v>
+        <v>0.161256132457</v>
       </c>
       <c r="AR17" t="n">
-        <v>-1.708229861</v>
+        <v>1.708229861</v>
       </c>
       <c r="AS17" t="n">
         <v>0.307202110753</v>
@@ -4033,10 +4033,10 @@
         <v>0.8881770785250003</v>
       </c>
       <c r="AW17" t="n">
-        <v>-1.708229861</v>
+        <v>1.708229861</v>
       </c>
       <c r="AX17" t="n">
-        <v>1.060896496556</v>
+        <v>4.638612351013</v>
       </c>
     </row>
     <row r="18">
@@ -4065,10 +4065,10 @@
         <v>0.002763499634968</v>
       </c>
       <c r="I18" t="n">
-        <v>100.6913959550503</v>
+        <v>99.3133515048704</v>
       </c>
       <c r="J18" t="n">
-        <v>1653.002498587735</v>
+        <v>1550.423723484218</v>
       </c>
       <c r="K18" t="n">
         <v>0.05418964317417199</v>
@@ -4083,10 +4083,10 @@
         <v>0.000147776130351</v>
       </c>
       <c r="O18" t="n">
-        <v>-1.910672469399976e-05</v>
+        <v>1.910672469399976e-05</v>
       </c>
       <c r="P18" t="n">
-        <v>-0.001727336585694</v>
+        <v>0.001727336585694</v>
       </c>
       <c r="Q18" t="n">
         <v>0.000560536184349</v>
@@ -4095,10 +4095,10 @@
         <v>0.001035953208876</v>
       </c>
       <c r="S18" t="n">
-        <v>-0.001727336585694</v>
+        <v>0.001727336585694</v>
       </c>
       <c r="T18" t="n">
-        <v>0.001036163049274</v>
+        <v>0.004509942945356</v>
       </c>
       <c r="U18" t="inlineStr">
         <is>
@@ -4116,49 +4116,49 @@
         </is>
       </c>
       <c r="X18" t="n">
-        <v>54189.643174172</v>
+        <v>45158.03597847666</v>
       </c>
       <c r="Y18" t="n">
-        <v>3622.35804</v>
+        <v>3018.6317</v>
       </c>
       <c r="Z18" t="n">
-        <v>3621.69448</v>
+        <v>3018.07873</v>
       </c>
       <c r="AA18" t="n">
-        <v>2763.499634968</v>
+        <v>2302.916362473333</v>
       </c>
       <c r="AB18" t="n">
-        <v>2782.606359662</v>
+        <v>2318.838633051666</v>
       </c>
       <c r="AC18" t="n">
-        <v>54189.64317417199</v>
+        <v>45158.03597847666</v>
       </c>
       <c r="AD18" t="n">
-        <v>52462.30658847799</v>
+        <v>43718.58882373167</v>
       </c>
       <c r="AE18" t="n">
-        <v>-19.10672469399976</v>
+        <v>15.92227057833313</v>
       </c>
       <c r="AF18" t="n">
-        <v>-1727.336585694</v>
+        <v>1439.447154745</v>
       </c>
       <c r="AG18" t="n">
-        <v>5.626722587999747</v>
+        <v>4.688935489999789</v>
       </c>
       <c r="AH18" t="n">
-        <v>147.776130351</v>
+        <v>123.1467752925</v>
       </c>
       <c r="AI18" t="n">
-        <v>560.536184349</v>
+        <v>467.1134869575</v>
       </c>
       <c r="AJ18" t="n">
-        <v>1035.953208876</v>
+        <v>863.2943407300003</v>
       </c>
       <c r="AK18" t="n">
-        <v>-1727.336585694</v>
+        <v>1439.447154745</v>
       </c>
       <c r="AL18" t="n">
-        <v>1036.163049274</v>
+        <v>3758.285787796666</v>
       </c>
       <c r="AM18" t="n">
         <v>2.763499634968</v>
@@ -4173,10 +4173,10 @@
         <v>52.46230658847799</v>
       </c>
       <c r="AQ18" t="n">
-        <v>-0.01910672469399976</v>
+        <v>0.01910672469399976</v>
       </c>
       <c r="AR18" t="n">
-        <v>-1.727336585694</v>
+        <v>1.727336585694</v>
       </c>
       <c r="AS18" t="n">
         <v>0.005626722587999747</v>
@@ -4191,10 +4191,10 @@
         <v>1.035953208876</v>
       </c>
       <c r="AW18" t="n">
-        <v>-1.727336585694</v>
+        <v>1.727336585694</v>
       </c>
       <c r="AX18" t="n">
-        <v>1.036163049274</v>
+        <v>4.509942945355999</v>
       </c>
     </row>
     <row r="19">
@@ -4223,10 +4223,10 @@
         <v>0.002754885572727</v>
       </c>
       <c r="I19" t="n">
-        <v>100.3644901708226</v>
+        <v>99.63683353524515</v>
       </c>
       <c r="J19" t="n">
-        <v>1753.366988758557</v>
+        <v>1650.060557019464</v>
       </c>
       <c r="K19" t="n">
         <v>0.05695457003402898</v>
@@ -4241,10 +4241,10 @@
         <v>1.767949980499995e-05</v>
       </c>
       <c r="O19" t="n">
-        <v>-1.004128713000003e-05</v>
+        <v>1.004128713000003e-05</v>
       </c>
       <c r="P19" t="n">
-        <v>-0.001737377872824</v>
+        <v>0.001737377872824</v>
       </c>
       <c r="Q19" t="n">
         <v>0.0005691502465900002</v>
@@ -4253,10 +4253,10 @@
         <v>0.001053632708681</v>
       </c>
       <c r="S19" t="n">
-        <v>-0.001737377872824</v>
+        <v>0.001737377872824</v>
       </c>
       <c r="T19" t="n">
-        <v>0.001017507699903</v>
+        <v>0.004502304732681</v>
       </c>
       <c r="U19" t="inlineStr">
         <is>
@@ -4274,49 +4274,49 @@
         </is>
       </c>
       <c r="X19" t="n">
-        <v>56954.570034029</v>
+        <v>47462.14169502416</v>
       </c>
       <c r="Y19" t="n">
-        <v>3622.39558</v>
+        <v>3018.66298</v>
       </c>
       <c r="Z19" t="n">
-        <v>3621.71754</v>
+        <v>3018.09795</v>
       </c>
       <c r="AA19" t="n">
-        <v>2754.885572727</v>
+        <v>2295.7379772725</v>
       </c>
       <c r="AB19" t="n">
-        <v>2764.926859857</v>
+        <v>2304.1057165475</v>
       </c>
       <c r="AC19" t="n">
-        <v>56954.57003402898</v>
+        <v>47462.14169502415</v>
       </c>
       <c r="AD19" t="n">
-        <v>55217.19216120499</v>
+        <v>46014.32680100416</v>
       </c>
       <c r="AE19" t="n">
-        <v>-10.04128713000003</v>
+        <v>8.367739275000023</v>
       </c>
       <c r="AF19" t="n">
-        <v>-1737.377872824</v>
+        <v>1447.81489402</v>
       </c>
       <c r="AG19" t="n">
-        <v>8.614062241000218</v>
+        <v>7.178385200833516</v>
       </c>
       <c r="AH19" t="n">
-        <v>17.67949980499995</v>
+        <v>14.73291650416663</v>
       </c>
       <c r="AI19" t="n">
-        <v>569.1502465900002</v>
+        <v>474.2918721583335</v>
       </c>
       <c r="AJ19" t="n">
-        <v>1053.632708681</v>
+        <v>878.0272572341669</v>
       </c>
       <c r="AK19" t="n">
-        <v>-1737.377872824</v>
+        <v>1447.81489402</v>
       </c>
       <c r="AL19" t="n">
-        <v>1017.507699903</v>
+        <v>3751.9206105675</v>
       </c>
       <c r="AM19" t="n">
         <v>2.754885572727</v>
@@ -4331,10 +4331,10 @@
         <v>55.21719216120499</v>
       </c>
       <c r="AQ19" t="n">
-        <v>-0.01004128713000003</v>
+        <v>0.01004128713000003</v>
       </c>
       <c r="AR19" t="n">
-        <v>-1.737377872824</v>
+        <v>1.737377872824</v>
       </c>
       <c r="AS19" t="n">
         <v>0.008614062241000219</v>
@@ -4349,10 +4349,10 @@
         <v>1.053632708681</v>
       </c>
       <c r="AW19" t="n">
-        <v>-1.737377872824</v>
+        <v>1.737377872824</v>
       </c>
       <c r="AX19" t="n">
-        <v>1.017507699903</v>
+        <v>4.502304732681</v>
       </c>
     </row>
     <row r="20">
@@ -4381,10 +4381,10 @@
         <v>0.002104310153263</v>
       </c>
       <c r="I20" t="n">
-        <v>116.2778299030138</v>
+        <v>86.00091701350895</v>
       </c>
       <c r="J20" t="n">
-        <v>1869.644818661571</v>
+        <v>1736.061474032973</v>
       </c>
       <c r="K20" t="n">
         <v>0.05940141621467199</v>
@@ -4399,10 +4399,10 @@
         <v>0.0003180806792139998</v>
       </c>
       <c r="O20" t="n">
-        <v>-0.0003425360273800002</v>
+        <v>0.0003425360273800002</v>
       </c>
       <c r="P20" t="n">
-        <v>-0.002079913900204</v>
+        <v>0.002079913900204</v>
       </c>
       <c r="Q20" t="n">
         <v>0.001219725666054</v>
@@ -4411,10 +4411,10 @@
         <v>0.001371713387895</v>
       </c>
       <c r="S20" t="n">
-        <v>-0.002079913900204</v>
+        <v>0.002079913900204</v>
       </c>
       <c r="T20" t="n">
-        <v>2.439625305899985e-05</v>
+        <v>0.004526760080847</v>
       </c>
       <c r="U20" t="inlineStr">
         <is>
@@ -4432,49 +4432,49 @@
         </is>
       </c>
       <c r="X20" t="n">
-        <v>59401.416214672</v>
+        <v>49501.18017889334</v>
       </c>
       <c r="Y20" t="n">
-        <v>7245.50586</v>
+        <v>6037.92155</v>
       </c>
       <c r="Z20" t="n">
-        <v>7244.4593</v>
+        <v>6037.04941</v>
       </c>
       <c r="AA20" t="n">
-        <v>2104.310153263</v>
+        <v>1753.591794385833</v>
       </c>
       <c r="AB20" t="n">
-        <v>2446.846180643</v>
+        <v>2039.038483869167</v>
       </c>
       <c r="AC20" t="n">
-        <v>59401.41621467199</v>
+        <v>49501.18017889332</v>
       </c>
       <c r="AD20" t="n">
-        <v>57321.50231446799</v>
+        <v>47767.91859538999</v>
       </c>
       <c r="AE20" t="n">
-        <v>-342.5360273800002</v>
+        <v>285.4466894833336</v>
       </c>
       <c r="AF20" t="n">
-        <v>-2079.913900204</v>
+        <v>1733.261583503333</v>
       </c>
       <c r="AG20" t="n">
-        <v>650.575419464</v>
+        <v>542.1461828866667</v>
       </c>
       <c r="AH20" t="n">
-        <v>318.0806792139998</v>
+        <v>265.0672326783332</v>
       </c>
       <c r="AI20" t="n">
-        <v>1219.725666054</v>
+        <v>1016.438055045</v>
       </c>
       <c r="AJ20" t="n">
-        <v>1371.713387895</v>
+        <v>1143.0944899125</v>
       </c>
       <c r="AK20" t="n">
-        <v>-2079.913900204</v>
+        <v>1733.261583503333</v>
       </c>
       <c r="AL20" t="n">
-        <v>24.39625305899985</v>
+        <v>3772.300067372501</v>
       </c>
       <c r="AM20" t="n">
         <v>2.104310153263</v>
@@ -4489,10 +4489,10 @@
         <v>57.32150231446799</v>
       </c>
       <c r="AQ20" t="n">
-        <v>-0.3425360273800002</v>
+        <v>0.3425360273800002</v>
       </c>
       <c r="AR20" t="n">
-        <v>-2.079913900204</v>
+        <v>2.079913900204</v>
       </c>
       <c r="AS20" t="n">
         <v>0.650575419464</v>
@@ -4507,10 +4507,10 @@
         <v>1.371713387895</v>
       </c>
       <c r="AW20" t="n">
-        <v>-2.079913900204</v>
+        <v>2.079913900204</v>
       </c>
       <c r="AX20" t="n">
-        <v>0.02439625305899985</v>
+        <v>4.526760080847001</v>
       </c>
     </row>
     <row r="21">
@@ -4539,10 +4539,10 @@
         <v>0.002087454966744</v>
       </c>
       <c r="I21" t="n">
-        <v>101.0329497448576</v>
+        <v>98.97761101950782</v>
       </c>
       <c r="J21" t="n">
-        <v>1970.677768406429</v>
+        <v>1835.03908505248</v>
       </c>
       <c r="K21" t="n">
         <v>0.06151043354216899</v>
@@ -4557,10 +4557,10 @@
         <v>0.0003378288531460001</v>
       </c>
       <c r="O21" t="n">
-        <v>-2.15623607530001e-05</v>
+        <v>2.15623607530001e-05</v>
       </c>
       <c r="P21" t="n">
-        <v>-0.002101476260957</v>
+        <v>0.002101476260957</v>
       </c>
       <c r="Q21" t="n">
         <v>0.001236580852573</v>
@@ -4569,10 +4569,10 @@
         <v>0.001709542241041</v>
       </c>
       <c r="S21" t="n">
-        <v>-0.002101476260957</v>
+        <v>0.002101476260957</v>
       </c>
       <c r="T21" t="n">
-        <v>-1.402129421300023e-05</v>
+        <v>0.004210493588454</v>
       </c>
       <c r="U21" t="inlineStr">
         <is>
@@ -4590,49 +4590,49 @@
         </is>
       </c>
       <c r="X21" t="n">
-        <v>61510.433542169</v>
+        <v>51258.69461847417</v>
       </c>
       <c r="Y21" t="n">
-        <v>7245.546</v>
+        <v>6037.955</v>
       </c>
       <c r="Z21" t="n">
-        <v>7244.4862</v>
+        <v>6037.07183</v>
       </c>
       <c r="AA21" t="n">
-        <v>2087.454966744</v>
+        <v>1739.54580562</v>
       </c>
       <c r="AB21" t="n">
-        <v>2109.017327497</v>
+        <v>1757.514439580833</v>
       </c>
       <c r="AC21" t="n">
-        <v>61510.43354216898</v>
+        <v>51258.69461847416</v>
       </c>
       <c r="AD21" t="n">
-        <v>59408.95728121199</v>
+        <v>49507.46440100999</v>
       </c>
       <c r="AE21" t="n">
-        <v>-21.5623607530001</v>
+        <v>17.96863396083342</v>
       </c>
       <c r="AF21" t="n">
-        <v>-2101.476260957</v>
+        <v>1751.230217464167</v>
       </c>
       <c r="AG21" t="n">
-        <v>16.85518651899998</v>
+        <v>14.04598876583332</v>
       </c>
       <c r="AH21" t="n">
-        <v>337.8288531460001</v>
+        <v>281.5240442883334</v>
       </c>
       <c r="AI21" t="n">
-        <v>1236.580852573</v>
+        <v>1030.484043810834</v>
       </c>
       <c r="AJ21" t="n">
-        <v>1709.542241041</v>
+        <v>1424.618534200834</v>
       </c>
       <c r="AK21" t="n">
-        <v>-2101.476260957</v>
+        <v>1751.230217464167</v>
       </c>
       <c r="AL21" t="n">
-        <v>-14.02129421300023</v>
+        <v>3508.744657045</v>
       </c>
       <c r="AM21" t="n">
         <v>2.087454966744</v>
@@ -4647,10 +4647,10 @@
         <v>59.40895728121199</v>
       </c>
       <c r="AQ21" t="n">
-        <v>-0.0215623607530001</v>
+        <v>0.0215623607530001</v>
       </c>
       <c r="AR21" t="n">
-        <v>-2.101476260957</v>
+        <v>2.101476260957</v>
       </c>
       <c r="AS21" t="n">
         <v>0.01685518651899998</v>
@@ -4665,10 +4665,10 @@
         <v>1.709542241041</v>
       </c>
       <c r="AW21" t="n">
-        <v>-2.101476260957</v>
+        <v>2.101476260957</v>
       </c>
       <c r="AX21" t="n">
-        <v>-0.01402129421300023</v>
+        <v>4.210493588454</v>
       </c>
     </row>
     <row r="22">
@@ -4697,10 +4697,10 @@
         <v>0.0020784126373</v>
       </c>
       <c r="I22" t="n">
-        <v>100.3232581035847</v>
+        <v>99.67778348740339</v>
       </c>
       <c r="J22" t="n">
-        <v>2071.001026510013</v>
+        <v>1934.716868539884</v>
       </c>
       <c r="K22" t="n">
         <v>0.06359556481674498</v>
@@ -4715,10 +4715,10 @@
         <v>2.388605292099992e-05</v>
       </c>
       <c r="O22" t="n">
-        <v>-6.718637275999941e-06</v>
+        <v>6.718637275999941e-06</v>
       </c>
       <c r="P22" t="n">
-        <v>-0.002108194898233</v>
+        <v>0.002108194898233</v>
       </c>
       <c r="Q22" t="n">
         <v>0.001245623182017</v>
@@ -4727,10 +4727,10 @@
         <v>0.001733428293962</v>
       </c>
       <c r="S22" t="n">
-        <v>-0.002108194898233</v>
+        <v>0.002108194898233</v>
       </c>
       <c r="T22" t="n">
-        <v>-2.978226093299993e-05</v>
+        <v>0.004193326172809</v>
       </c>
       <c r="U22" t="inlineStr">
         <is>
@@ -4748,49 +4748,49 @@
         </is>
       </c>
       <c r="X22" t="n">
-        <v>63595.564816745</v>
+        <v>52996.30401395416</v>
       </c>
       <c r="Y22" t="n">
-        <v>7245.52549</v>
+        <v>6037.93791</v>
       </c>
       <c r="Z22" t="n">
-        <v>7244.48024</v>
+        <v>6037.06686</v>
       </c>
       <c r="AA22" t="n">
-        <v>2078.4126373</v>
+        <v>1732.010531083333</v>
       </c>
       <c r="AB22" t="n">
-        <v>2085.131274576</v>
+        <v>1737.60939548</v>
       </c>
       <c r="AC22" t="n">
-        <v>63595.56481674498</v>
+        <v>52996.30401395416</v>
       </c>
       <c r="AD22" t="n">
-        <v>61487.36991851199</v>
+        <v>51239.47493209333</v>
       </c>
       <c r="AE22" t="n">
-        <v>-6.718637275999941</v>
+        <v>5.598864396666618</v>
       </c>
       <c r="AF22" t="n">
-        <v>-2108.194898233</v>
+        <v>1756.829081860833</v>
       </c>
       <c r="AG22" t="n">
-        <v>9.042329443999762</v>
+        <v>7.535274536666469</v>
       </c>
       <c r="AH22" t="n">
-        <v>23.88605292099992</v>
+        <v>19.90504410083327</v>
       </c>
       <c r="AI22" t="n">
-        <v>1245.623182017</v>
+        <v>1038.0193183475</v>
       </c>
       <c r="AJ22" t="n">
-        <v>1733.428293962</v>
+        <v>1444.523578301667</v>
       </c>
       <c r="AK22" t="n">
-        <v>-2108.194898233</v>
+        <v>1756.829081860833</v>
       </c>
       <c r="AL22" t="n">
-        <v>-29.78226093299993</v>
+        <v>3494.438477340834</v>
       </c>
       <c r="AM22" t="n">
         <v>2.0784126373</v>
@@ -4805,10 +4805,10 @@
         <v>61.48736991851199</v>
       </c>
       <c r="AQ22" t="n">
-        <v>-0.006718637275999941</v>
+        <v>0.006718637275999941</v>
       </c>
       <c r="AR22" t="n">
-        <v>-2.108194898233</v>
+        <v>2.108194898233</v>
       </c>
       <c r="AS22" t="n">
         <v>0.009042329443999762</v>
@@ -4823,10 +4823,10 @@
         <v>1.733428293962</v>
       </c>
       <c r="AW22" t="n">
-        <v>-2.108194898233</v>
+        <v>2.108194898233</v>
       </c>
       <c r="AX22" t="n">
-        <v>-0.02978226093299993</v>
+        <v>4.193326172809001</v>
       </c>
     </row>
     <row r="23">
@@ -4855,10 +4855,10 @@
         <v>0.003330624942127</v>
       </c>
       <c r="I23" t="n">
-        <v>84.99036020120761</v>
+        <v>117.6604026189068</v>
       </c>
       <c r="J23" t="n">
-        <v>2155.991386711221</v>
+        <v>2052.377271158791</v>
       </c>
       <c r="K23" t="n">
         <v>0.06642627495200998</v>
@@ -4873,10 +4873,10 @@
         <v>-0.0007455788606889999</v>
       </c>
       <c r="O23" t="n">
-        <v>0.0004999148068620001</v>
+        <v>-0.0004999148068620001</v>
       </c>
       <c r="P23" t="n">
-        <v>-0.001608280091371</v>
+        <v>0.001608280091371</v>
       </c>
       <c r="Q23" t="n">
         <v>-6.589122810000004e-06</v>
@@ -4885,10 +4885,10 @@
         <v>0.0009878494332730002</v>
       </c>
       <c r="S23" t="n">
-        <v>-0.001608280091371</v>
+        <v>0.001608280091371</v>
       </c>
       <c r="T23" t="n">
-        <v>0.001722344850756</v>
+        <v>0.004438990226636</v>
       </c>
       <c r="U23" t="inlineStr">
         <is>
@@ -4906,49 +4906,49 @@
         </is>
       </c>
       <c r="X23" t="n">
-        <v>66426.27495200999</v>
+        <v>55355.229126675</v>
       </c>
       <c r="Y23" t="n">
-        <v>180.84394</v>
+        <v>150.70329</v>
       </c>
       <c r="Z23" t="n">
-        <v>180.49688</v>
+        <v>150.41406</v>
       </c>
       <c r="AA23" t="n">
-        <v>3330.624942127</v>
+        <v>2775.520785105834</v>
       </c>
       <c r="AB23" t="n">
-        <v>2830.710135265</v>
+        <v>2358.925112720834</v>
       </c>
       <c r="AC23" t="n">
-        <v>66426.27495200998</v>
+        <v>55355.22912667498</v>
       </c>
       <c r="AD23" t="n">
-        <v>64817.994860639</v>
+        <v>54014.99571719916</v>
       </c>
       <c r="AE23" t="n">
-        <v>499.9148068620001</v>
+        <v>-416.5956723850001</v>
       </c>
       <c r="AF23" t="n">
-        <v>-1608.280091371</v>
+        <v>1340.233409475833</v>
       </c>
       <c r="AG23" t="n">
-        <v>-1252.212304827</v>
+        <v>-1043.5102540225</v>
       </c>
       <c r="AH23" t="n">
-        <v>-745.5788606889998</v>
+        <v>-621.3157172408332</v>
       </c>
       <c r="AI23" t="n">
-        <v>-6.589122810000004</v>
+        <v>-5.490935675000004</v>
       </c>
       <c r="AJ23" t="n">
-        <v>987.8494332730003</v>
+        <v>823.2078610608336</v>
       </c>
       <c r="AK23" t="n">
-        <v>-1608.280091371</v>
+        <v>1340.233409475833</v>
       </c>
       <c r="AL23" t="n">
-        <v>1722.344850756</v>
+        <v>3699.158522196667</v>
       </c>
       <c r="AM23" t="n">
         <v>3.330624942127</v>
@@ -4963,10 +4963,10 @@
         <v>64.81799486063899</v>
       </c>
       <c r="AQ23" t="n">
-        <v>0.4999148068620001</v>
+        <v>-0.4999148068620001</v>
       </c>
       <c r="AR23" t="n">
-        <v>-1.608280091371</v>
+        <v>1.608280091371</v>
       </c>
       <c r="AS23" t="n">
         <v>-1.252212304827</v>
@@ -4981,10 +4981,10 @@
         <v>0.9878494332730002</v>
       </c>
       <c r="AW23" t="n">
-        <v>-1.608280091371</v>
+        <v>1.608280091371</v>
       </c>
       <c r="AX23" t="n">
-        <v>1.722344850756</v>
+        <v>4.438990226636</v>
       </c>
     </row>
     <row r="24">
@@ -5013,10 +5013,10 @@
         <v>0.00334164728746</v>
       </c>
       <c r="I24" t="n">
-        <v>102.9170832444765</v>
+        <v>97.16559860373512</v>
       </c>
       <c r="J24" t="n">
-        <v>2258.908469955697</v>
+        <v>2149.542869762526</v>
       </c>
       <c r="K24" t="n">
         <v>0.06986540087258197</v>
@@ -5031,10 +5031,10 @@
         <v>-0.0006084157853070002</v>
       </c>
       <c r="O24" t="n">
-        <v>-9.747863311200013e-05</v>
+        <v>9.747863311200013e-05</v>
       </c>
       <c r="P24" t="n">
-        <v>-0.001705758724483</v>
+        <v>0.001705758724483</v>
       </c>
       <c r="Q24" t="n">
         <v>-1.76114681429999e-05</v>
@@ -5043,10 +5043,10 @@
         <v>0.0003794336479660001</v>
       </c>
       <c r="S24" t="n">
-        <v>-0.001705758724483</v>
+        <v>0.001705758724483</v>
       </c>
       <c r="T24" t="n">
-        <v>0.001635888562977</v>
+        <v>0.005144884645055</v>
       </c>
       <c r="U24" t="inlineStr">
         <is>
@@ -5064,49 +5064,49 @@
         </is>
       </c>
       <c r="X24" t="n">
-        <v>69865.40087258199</v>
+        <v>58221.16739381832</v>
       </c>
       <c r="Y24" t="n">
-        <v>180.86547</v>
+        <v>150.72122</v>
       </c>
       <c r="Z24" t="n">
-        <v>180.48729</v>
+        <v>150.40608</v>
       </c>
       <c r="AA24" t="n">
-        <v>3341.64728746</v>
+        <v>2784.706072883333</v>
       </c>
       <c r="AB24" t="n">
-        <v>3439.125920572</v>
+        <v>2865.938267143334</v>
       </c>
       <c r="AC24" t="n">
-        <v>69865.40087258197</v>
+        <v>58221.16739381832</v>
       </c>
       <c r="AD24" t="n">
-        <v>68159.642148099</v>
+        <v>56799.7017900825</v>
       </c>
       <c r="AE24" t="n">
-        <v>-97.47863311200013</v>
+        <v>81.23219426000011</v>
       </c>
       <c r="AF24" t="n">
-        <v>-1705.758724483</v>
+        <v>1421.465603735833</v>
       </c>
       <c r="AG24" t="n">
-        <v>-11.0223453329999</v>
+        <v>-9.185287777499916</v>
       </c>
       <c r="AH24" t="n">
-        <v>-608.4157853070002</v>
+        <v>-507.0131544225002</v>
       </c>
       <c r="AI24" t="n">
-        <v>-17.6114681429999</v>
+        <v>-14.67622345249992</v>
       </c>
       <c r="AJ24" t="n">
-        <v>379.4336479660001</v>
+        <v>316.1947066383334</v>
       </c>
       <c r="AK24" t="n">
-        <v>-1705.758724483</v>
+        <v>1421.465603735833</v>
       </c>
       <c r="AL24" t="n">
-        <v>1635.888562977</v>
+        <v>4287.403870879167</v>
       </c>
       <c r="AM24" t="n">
         <v>3.34164728746</v>
@@ -5121,10 +5121,10 @@
         <v>68.159642148099</v>
       </c>
       <c r="AQ24" t="n">
-        <v>-0.09747863311200013</v>
+        <v>0.09747863311200013</v>
       </c>
       <c r="AR24" t="n">
-        <v>-1.705758724483</v>
+        <v>1.705758724483</v>
       </c>
       <c r="AS24" t="n">
         <v>-0.0110223453329999</v>
@@ -5139,10 +5139,10 @@
         <v>0.379433647966</v>
       </c>
       <c r="AW24" t="n">
-        <v>-1.705758724483</v>
+        <v>1.705758724483</v>
       </c>
       <c r="AX24" t="n">
-        <v>1.635888562977</v>
+        <v>5.144884645055</v>
       </c>
     </row>
     <row r="25">
@@ -5171,10 +5171,10 @@
         <v>0.003344291836583</v>
       </c>
       <c r="I25" t="n">
-        <v>103.1716053801804</v>
+        <v>96.92589315781872</v>
       </c>
       <c r="J25" t="n">
-        <v>2362.080075335878</v>
+        <v>2246.468762920344</v>
       </c>
       <c r="K25" t="n">
         <v>0.07331576044898297</v>
@@ -5189,10 +5189,10 @@
         <v>-1.123365582899986e-05</v>
       </c>
       <c r="O25" t="n">
-        <v>-0.0001060677398179999</v>
+        <v>0.0001060677398179999</v>
       </c>
       <c r="P25" t="n">
-        <v>-0.001811826464301</v>
+        <v>0.001811826464301</v>
       </c>
       <c r="Q25" t="n">
         <v>-2.025601726600001e-05</v>
@@ -5201,10 +5201,10 @@
         <v>0.0003681999921370002</v>
       </c>
       <c r="S25" t="n">
-        <v>-0.001811826464301</v>
+        <v>0.001811826464301</v>
       </c>
       <c r="T25" t="n">
-        <v>0.001532465372282</v>
+        <v>0.005262186040701999</v>
       </c>
       <c r="U25" t="inlineStr">
         <is>
@@ -5222,49 +5222,49 @@
         </is>
       </c>
       <c r="X25" t="n">
-        <v>73315.76044898298</v>
+        <v>61096.46704081915</v>
       </c>
       <c r="Y25" t="n">
-        <v>180.87537</v>
+        <v>150.72947</v>
       </c>
       <c r="Z25" t="n">
-        <v>180.50665</v>
+        <v>150.4222</v>
       </c>
       <c r="AA25" t="n">
-        <v>3344.291836583</v>
+        <v>2786.909863819167</v>
       </c>
       <c r="AB25" t="n">
-        <v>3450.359576401</v>
+        <v>2875.299647000833</v>
       </c>
       <c r="AC25" t="n">
-        <v>73315.76044898297</v>
+        <v>61096.46704081915</v>
       </c>
       <c r="AD25" t="n">
-        <v>71503.93398468199</v>
+        <v>59586.61165390167</v>
       </c>
       <c r="AE25" t="n">
-        <v>-106.0677398179999</v>
+        <v>88.38978318166657</v>
       </c>
       <c r="AF25" t="n">
-        <v>-1811.826464301</v>
+        <v>1509.8553869175</v>
       </c>
       <c r="AG25" t="n">
-        <v>-2.644549123000106</v>
+        <v>-2.203790935833422</v>
       </c>
       <c r="AH25" t="n">
-        <v>-11.23365582899986</v>
+        <v>-9.361379857499887</v>
       </c>
       <c r="AI25" t="n">
-        <v>-20.25601726600001</v>
+        <v>-16.88001438833334</v>
       </c>
       <c r="AJ25" t="n">
-        <v>368.1999921370002</v>
+        <v>306.8333267808335</v>
       </c>
       <c r="AK25" t="n">
-        <v>-1811.826464301</v>
+        <v>1509.8553869175</v>
       </c>
       <c r="AL25" t="n">
-        <v>1532.465372282</v>
+        <v>4385.155033918333</v>
       </c>
       <c r="AM25" t="n">
         <v>3.344291836583</v>
@@ -5279,10 +5279,10 @@
         <v>71.50393398468199</v>
       </c>
       <c r="AQ25" t="n">
-        <v>-0.1060677398179999</v>
+        <v>0.1060677398179999</v>
       </c>
       <c r="AR25" t="n">
-        <v>-1.811826464301</v>
+        <v>1.811826464301</v>
       </c>
       <c r="AS25" t="n">
         <v>-0.002644549123000106</v>
@@ -5297,10 +5297,10 @@
         <v>0.3681999921370002</v>
       </c>
       <c r="AW25" t="n">
-        <v>-1.811826464301</v>
+        <v>1.811826464301</v>
       </c>
       <c r="AX25" t="n">
-        <v>1.532465372282</v>
+        <v>5.262186040702</v>
       </c>
     </row>
   </sheetData>
@@ -6002,7 +6002,7 @@
         <v>0</v>
       </c>
       <c r="BI3" t="n">
-        <v>2.10949</v>
+        <v>1.75791</v>
       </c>
       <c r="BJ3" t="inlineStr">
         <is>
@@ -6194,7 +6194,7 @@
         <v>0</v>
       </c>
       <c r="BI4" t="n">
-        <v>180.83741</v>
+        <v>150.69784</v>
       </c>
       <c r="BJ4" t="inlineStr">
         <is>
@@ -6386,7 +6386,7 @@
         <v>0</v>
       </c>
       <c r="BI5" t="n">
-        <v>72.46127</v>
+        <v>60.38439</v>
       </c>
       <c r="BJ5" t="inlineStr">
         <is>
@@ -6562,7 +6562,7 @@
         <v>0</v>
       </c>
       <c r="BI6" t="n">
-        <v>0.34966</v>
+        <v>0.29138</v>
       </c>
       <c r="BJ6" t="inlineStr">
         <is>
@@ -6946,7 +6946,7 @@
         <v>0</v>
       </c>
       <c r="BI8" t="n">
-        <v>180.47164</v>
+        <v>150.39303</v>
       </c>
       <c r="BJ8" t="inlineStr">
         <is>
@@ -7138,7 +7138,7 @@
         <v>0</v>
       </c>
       <c r="BI9" t="n">
-        <v>72.45263</v>
+        <v>60.37719</v>
       </c>
       <c r="BJ9" t="inlineStr">
         <is>
@@ -7314,7 +7314,7 @@
         <v>0</v>
       </c>
       <c r="BI10" t="n">
-        <v>0.35296</v>
+        <v>0.29413</v>
       </c>
       <c r="BJ10" t="inlineStr">
         <is>
@@ -7698,7 +7698,7 @@
         <v>0</v>
       </c>
       <c r="BI12" t="n">
-        <v>180.84679</v>
+        <v>150.70566</v>
       </c>
       <c r="BJ12" t="inlineStr">
         <is>
@@ -7890,7 +7890,7 @@
         <v>0</v>
       </c>
       <c r="BI13" t="n">
-        <v>72.46099</v>
+        <v>60.38415</v>
       </c>
       <c r="BJ13" t="inlineStr">
         <is>
@@ -8066,7 +8066,7 @@
         <v>0</v>
       </c>
       <c r="BI14" t="n">
-        <v>0.00165</v>
+        <v>0.00138</v>
       </c>
       <c r="BJ14" t="inlineStr">
         <is>
@@ -8450,7 +8450,7 @@
         <v>0</v>
       </c>
       <c r="BI16" t="n">
-        <v>180.48534</v>
+        <v>150.40445</v>
       </c>
       <c r="BJ16" t="inlineStr">
         <is>
@@ -8642,7 +8642,7 @@
         <v>0</v>
       </c>
       <c r="BI17" t="n">
-        <v>72.45277</v>
+        <v>60.37731</v>
       </c>
       <c r="BJ17" t="inlineStr">
         <is>
@@ -8818,7 +8818,7 @@
         <v>0</v>
       </c>
       <c r="BI18" t="n">
-        <v>0.35296</v>
+        <v>0.29413</v>
       </c>
       <c r="BJ18" t="inlineStr">
         <is>
@@ -9586,7 +9586,7 @@
         <v>0</v>
       </c>
       <c r="BI22" t="n">
-        <v>724.6024200000001</v>
+        <v>603.8353499999999</v>
       </c>
       <c r="BJ22" t="inlineStr">
         <is>
@@ -9954,7 +9954,7 @@
         <v>0</v>
       </c>
       <c r="BI24" t="n">
-        <v>0.34966</v>
+        <v>0.29138</v>
       </c>
       <c r="BJ24" t="inlineStr">
         <is>
@@ -10338,7 +10338,7 @@
         <v>0</v>
       </c>
       <c r="BI26" t="n">
-        <v>724.12467</v>
+        <v>603.43722</v>
       </c>
       <c r="BJ26" t="inlineStr">
         <is>
@@ -10706,7 +10706,7 @@
         <v>0</v>
       </c>
       <c r="BI28" t="n">
-        <v>0.00165</v>
+        <v>0.00138</v>
       </c>
       <c r="BJ28" t="inlineStr">
         <is>
@@ -11282,7 +11282,7 @@
         <v>0</v>
       </c>
       <c r="BI31" t="n">
-        <v>724.62012</v>
+        <v>603.8501</v>
       </c>
       <c r="BJ31" t="inlineStr">
         <is>
@@ -11650,7 +11650,7 @@
         <v>0</v>
       </c>
       <c r="BI33" t="n">
-        <v>0.34966</v>
+        <v>0.29138</v>
       </c>
       <c r="BJ33" t="inlineStr">
         <is>
@@ -12034,7 +12034,7 @@
         <v>0</v>
       </c>
       <c r="BI35" t="n">
-        <v>724.1258</v>
+        <v>603.43817</v>
       </c>
       <c r="BJ35" t="inlineStr">
         <is>
@@ -12402,7 +12402,7 @@
         <v>0</v>
       </c>
       <c r="BI37" t="n">
-        <v>0.35296</v>
+        <v>0.29413</v>
       </c>
       <c r="BJ37" t="inlineStr">
         <is>
@@ -12962,7 +12962,7 @@
         <v>0</v>
       </c>
       <c r="BI40" t="n">
-        <v>2.81211</v>
+        <v>2.34342</v>
       </c>
       <c r="BJ40" t="inlineStr">
         <is>
@@ -13154,7 +13154,7 @@
         <v>-100</v>
       </c>
       <c r="BI41" t="n">
-        <v>180.84716</v>
+        <v>150.70596</v>
       </c>
       <c r="BJ41" t="inlineStr">
         <is>
@@ -13330,7 +13330,7 @@
         <v>0</v>
       </c>
       <c r="BI42" t="n">
-        <v>0.00165</v>
+        <v>0.00138</v>
       </c>
       <c r="BJ42" t="inlineStr">
         <is>
@@ -13714,7 +13714,7 @@
         <v>0</v>
       </c>
       <c r="BI44" t="n">
-        <v>180.45366</v>
+        <v>150.37805</v>
       </c>
       <c r="BJ44" t="inlineStr">
         <is>
@@ -13890,7 +13890,7 @@
         <v>0</v>
       </c>
       <c r="BI45" t="n">
-        <v>0.35296</v>
+        <v>0.29413</v>
       </c>
       <c r="BJ45" t="inlineStr">
         <is>
@@ -14274,7 +14274,7 @@
         <v>0</v>
       </c>
       <c r="BI47" t="n">
-        <v>180.85294</v>
+        <v>150.71078</v>
       </c>
       <c r="BJ47" t="inlineStr">
         <is>
@@ -14450,7 +14450,7 @@
         <v>0</v>
       </c>
       <c r="BI48" t="n">
-        <v>0.34966</v>
+        <v>0.29138</v>
       </c>
       <c r="BJ48" t="inlineStr">
         <is>
@@ -14834,7 +14834,7 @@
         <v>0</v>
       </c>
       <c r="BI50" t="n">
-        <v>180.4316</v>
+        <v>150.35966</v>
       </c>
       <c r="BJ50" t="inlineStr">
         <is>
@@ -15010,7 +15010,7 @@
         <v>0</v>
       </c>
       <c r="BI51" t="n">
-        <v>0.00165</v>
+        <v>0.00138</v>
       </c>
       <c r="BJ51" t="inlineStr">
         <is>
@@ -15394,7 +15394,7 @@
         <v>0</v>
       </c>
       <c r="BI53" t="n">
-        <v>180.84635</v>
+        <v>150.70529</v>
       </c>
       <c r="BJ53" t="inlineStr">
         <is>
@@ -15570,7 +15570,7 @@
         <v>0</v>
       </c>
       <c r="BI54" t="n">
-        <v>0.35296</v>
+        <v>0.29413</v>
       </c>
       <c r="BJ54" t="inlineStr">
         <is>
@@ -15954,7 +15954,7 @@
         <v>0</v>
       </c>
       <c r="BI56" t="n">
-        <v>180.53224</v>
+        <v>150.44354</v>
       </c>
       <c r="BJ56" t="inlineStr">
         <is>
@@ -16130,7 +16130,7 @@
         <v>0</v>
       </c>
       <c r="BI57" t="n">
-        <v>0.35296</v>
+        <v>0.29413</v>
       </c>
       <c r="BJ57" t="inlineStr">
         <is>
@@ -16514,7 +16514,7 @@
         <v>0</v>
       </c>
       <c r="BI59" t="n">
-        <v>363.04386</v>
+        <v>302.53655</v>
       </c>
       <c r="BJ59" t="inlineStr">
         <is>
@@ -16690,7 +16690,7 @@
         <v>0</v>
       </c>
       <c r="BI60" t="n">
-        <v>0.00165</v>
+        <v>0.00138</v>
       </c>
       <c r="BJ60" t="inlineStr">
         <is>
@@ -17074,7 +17074,7 @@
         <v>0</v>
       </c>
       <c r="BI62" t="n">
-        <v>362.66427</v>
+        <v>302.22022</v>
       </c>
       <c r="BJ62" t="inlineStr">
         <is>
@@ -17250,7 +17250,7 @@
         <v>0</v>
       </c>
       <c r="BI63" t="n">
-        <v>0.00165</v>
+        <v>0.00138</v>
       </c>
       <c r="BJ63" t="inlineStr">
         <is>
@@ -17634,7 +17634,7 @@
         <v>0</v>
       </c>
       <c r="BI65" t="n">
-        <v>363.09642</v>
+        <v>302.58035</v>
       </c>
       <c r="BJ65" t="inlineStr">
         <is>
@@ -17810,7 +17810,7 @@
         <v>0</v>
       </c>
       <c r="BI66" t="n">
-        <v>0.34966</v>
+        <v>0.29138</v>
       </c>
       <c r="BJ66" t="inlineStr">
         <is>
@@ -18194,7 +18194,7 @@
         <v>0</v>
       </c>
       <c r="BI68" t="n">
-        <v>362.66394</v>
+        <v>302.21995</v>
       </c>
       <c r="BJ68" t="inlineStr">
         <is>
@@ -18370,7 +18370,7 @@
         <v>0</v>
       </c>
       <c r="BI69" t="n">
-        <v>0.34966</v>
+        <v>0.29138</v>
       </c>
       <c r="BJ69" t="inlineStr">
         <is>
@@ -18754,7 +18754,7 @@
         <v>0</v>
       </c>
       <c r="BI71" t="n">
-        <v>363.04371</v>
+        <v>302.53642</v>
       </c>
       <c r="BJ71" t="inlineStr">
         <is>
@@ -18930,7 +18930,7 @@
         <v>0</v>
       </c>
       <c r="BI72" t="n">
-        <v>0.34966</v>
+        <v>0.29138</v>
       </c>
       <c r="BJ72" t="inlineStr">
         <is>
@@ -19314,7 +19314,7 @@
         <v>0</v>
       </c>
       <c r="BI74" t="n">
-        <v>362.68092</v>
+        <v>302.2341</v>
       </c>
       <c r="BJ74" t="inlineStr">
         <is>
@@ -19490,7 +19490,7 @@
         <v>0</v>
       </c>
       <c r="BI75" t="n">
-        <v>0.00165</v>
+        <v>0.00138</v>
       </c>
       <c r="BJ75" t="inlineStr">
         <is>
@@ -19858,7 +19858,7 @@
         <v>0</v>
       </c>
       <c r="BI77" t="n">
-        <v>1.40688</v>
+        <v>1.1724</v>
       </c>
       <c r="BJ77" t="inlineStr">
         <is>
@@ -20050,7 +20050,7 @@
         <v>0</v>
       </c>
       <c r="BI78" t="n">
-        <v>724.67096</v>
+        <v>603.89246</v>
       </c>
       <c r="BJ78" t="inlineStr">
         <is>
@@ -20226,7 +20226,7 @@
         <v>0</v>
       </c>
       <c r="BI79" t="n">
-        <v>0.34966</v>
+        <v>0.29138</v>
       </c>
       <c r="BJ79" t="inlineStr">
         <is>
@@ -20610,7 +20610,7 @@
         <v>0</v>
       </c>
       <c r="BI81" t="n">
-        <v>724.17243</v>
+        <v>603.47702</v>
       </c>
       <c r="BJ81" t="inlineStr">
         <is>
@@ -20786,7 +20786,7 @@
         <v>0</v>
       </c>
       <c r="BI82" t="n">
-        <v>0.35296</v>
+        <v>0.29413</v>
       </c>
       <c r="BJ82" t="inlineStr">
         <is>
@@ -21170,7 +21170,7 @@
         <v>0</v>
       </c>
       <c r="BI84" t="n">
-        <v>724.70708</v>
+        <v>603.92257</v>
       </c>
       <c r="BJ84" t="inlineStr">
         <is>
@@ -21346,7 +21346,7 @@
         <v>0</v>
       </c>
       <c r="BI85" t="n">
-        <v>0.00165</v>
+        <v>0.00138</v>
       </c>
       <c r="BJ85" t="inlineStr">
         <is>
@@ -21730,7 +21730,7 @@
         <v>0</v>
       </c>
       <c r="BI87" t="n">
-        <v>724.1222299999999</v>
+        <v>603.43519</v>
       </c>
       <c r="BJ87" t="inlineStr">
         <is>
@@ -21906,7 +21906,7 @@
         <v>0</v>
       </c>
       <c r="BI88" t="n">
-        <v>0.35296</v>
+        <v>0.29413</v>
       </c>
       <c r="BJ88" t="inlineStr">
         <is>
@@ -22290,7 +22290,7 @@
         <v>0</v>
       </c>
       <c r="BI90" t="n">
-        <v>724.6967</v>
+        <v>603.91391</v>
       </c>
       <c r="BJ90" t="inlineStr">
         <is>
@@ -22466,7 +22466,7 @@
         <v>0</v>
       </c>
       <c r="BI91" t="n">
-        <v>0.00165</v>
+        <v>0.00138</v>
       </c>
       <c r="BJ91" t="inlineStr">
         <is>
@@ -22850,7 +22850,7 @@
         <v>0</v>
       </c>
       <c r="BI93" t="n">
-        <v>724.05727</v>
+        <v>603.38106</v>
       </c>
       <c r="BJ93" t="inlineStr">
         <is>
@@ -23026,7 +23026,7 @@
         <v>0</v>
       </c>
       <c r="BI94" t="n">
-        <v>0.35296</v>
+        <v>0.29413</v>
       </c>
       <c r="BJ94" t="inlineStr">
         <is>
@@ -23410,7 +23410,7 @@
         <v>0</v>
       </c>
       <c r="BI96" t="n">
-        <v>1811.74501</v>
+        <v>1509.78751</v>
       </c>
       <c r="BJ96" t="inlineStr">
         <is>
@@ -23586,7 +23586,7 @@
         <v>0</v>
       </c>
       <c r="BI97" t="n">
-        <v>0.34966</v>
+        <v>0.29138</v>
       </c>
       <c r="BJ97" t="inlineStr">
         <is>
@@ -23970,7 +23970,7 @@
         <v>0</v>
       </c>
       <c r="BI99" t="n">
-        <v>1810.94712</v>
+        <v>1509.1226</v>
       </c>
       <c r="BJ99" t="inlineStr">
         <is>
@@ -24146,7 +24146,7 @@
         <v>0</v>
       </c>
       <c r="BI100" t="n">
-        <v>0.35296</v>
+        <v>0.29413</v>
       </c>
       <c r="BJ100" t="inlineStr">
         <is>
@@ -24530,7 +24530,7 @@
         <v>0</v>
       </c>
       <c r="BI102" t="n">
-        <v>3622.37158</v>
+        <v>3018.64298</v>
       </c>
       <c r="BJ102" t="inlineStr">
         <is>
@@ -24706,7 +24706,7 @@
         <v>0</v>
       </c>
       <c r="BI103" t="n">
-        <v>1.05227</v>
+        <v>0.8768899999999999</v>
       </c>
       <c r="BJ103" t="inlineStr">
         <is>
@@ -25090,7 +25090,7 @@
         <v>0</v>
       </c>
       <c r="BI105" t="n">
-        <v>3621.68782</v>
+        <v>3018.07319</v>
       </c>
       <c r="BJ105" t="inlineStr">
         <is>
@@ -25266,7 +25266,7 @@
         <v>0</v>
       </c>
       <c r="BI106" t="n">
-        <v>1.75819</v>
+        <v>1.46516</v>
       </c>
       <c r="BJ106" t="inlineStr">
         <is>
@@ -25650,7 +25650,7 @@
         <v>0</v>
       </c>
       <c r="BI108" t="n">
-        <v>3622.35804</v>
+        <v>3018.6317</v>
       </c>
       <c r="BJ108" t="inlineStr">
         <is>
@@ -25826,7 +25826,7 @@
         <v>0</v>
       </c>
       <c r="BI109" t="n">
-        <v>1.40358</v>
+        <v>1.16965</v>
       </c>
       <c r="BJ109" t="inlineStr">
         <is>
@@ -26210,7 +26210,7 @@
         <v>0</v>
       </c>
       <c r="BI111" t="n">
-        <v>3621.69448</v>
+        <v>3018.07873</v>
       </c>
       <c r="BJ111" t="inlineStr">
         <is>
@@ -26386,7 +26386,7 @@
         <v>0</v>
       </c>
       <c r="BI112" t="n">
-        <v>2.4608</v>
+        <v>2.05067</v>
       </c>
       <c r="BJ112" t="inlineStr">
         <is>
@@ -26770,7 +26770,7 @@
         <v>0</v>
       </c>
       <c r="BI114" t="n">
-        <v>3622.39558</v>
+        <v>3018.66298</v>
       </c>
       <c r="BJ114" t="inlineStr">
         <is>
@@ -26946,7 +26946,7 @@
         <v>0</v>
       </c>
       <c r="BI115" t="n">
-        <v>0.70096</v>
+        <v>0.58414</v>
       </c>
       <c r="BJ115" t="inlineStr">
         <is>
@@ -27330,7 +27330,7 @@
         <v>0</v>
       </c>
       <c r="BI117" t="n">
-        <v>3621.71754</v>
+        <v>3018.09795</v>
       </c>
       <c r="BJ117" t="inlineStr">
         <is>
@@ -27506,7 +27506,7 @@
         <v>0</v>
       </c>
       <c r="BI118" t="n">
-        <v>1.40688</v>
+        <v>1.1724</v>
       </c>
       <c r="BJ118" t="inlineStr">
         <is>
@@ -27890,7 +27890,7 @@
         <v>0</v>
       </c>
       <c r="BI120" t="n">
-        <v>7245.50586</v>
+        <v>6037.92155</v>
       </c>
       <c r="BJ120" t="inlineStr">
         <is>
@@ -28066,7 +28066,7 @@
         <v>0</v>
       </c>
       <c r="BI121" t="n">
-        <v>1.75489</v>
+        <v>1.4624</v>
       </c>
       <c r="BJ121" t="inlineStr">
         <is>
@@ -28450,7 +28450,7 @@
         <v>0</v>
       </c>
       <c r="BI123" t="n">
-        <v>7244.4593</v>
+        <v>6037.04941</v>
       </c>
       <c r="BJ123" t="inlineStr">
         <is>
@@ -28626,7 +28626,7 @@
         <v>0</v>
       </c>
       <c r="BI124" t="n">
-        <v>2.81211</v>
+        <v>2.34342</v>
       </c>
       <c r="BJ124" t="inlineStr">
         <is>
@@ -29010,7 +29010,7 @@
         <v>0</v>
       </c>
       <c r="BI126" t="n">
-        <v>7245.546</v>
+        <v>6037.955</v>
       </c>
       <c r="BJ126" t="inlineStr">
         <is>
@@ -29186,7 +29186,7 @@
         <v>0</v>
       </c>
       <c r="BI127" t="n">
-        <v>0.70096</v>
+        <v>0.58414</v>
       </c>
       <c r="BJ127" t="inlineStr">
         <is>
@@ -29570,7 +29570,7 @@
         <v>0</v>
       </c>
       <c r="BI129" t="n">
-        <v>7244.4862</v>
+        <v>6037.07183</v>
       </c>
       <c r="BJ129" t="inlineStr">
         <is>
@@ -29746,7 +29746,7 @@
         <v>0</v>
       </c>
       <c r="BI130" t="n">
-        <v>3.86603</v>
+        <v>3.22169</v>
       </c>
       <c r="BJ130" t="inlineStr">
         <is>
@@ -30130,7 +30130,7 @@
         <v>0</v>
       </c>
       <c r="BI132" t="n">
-        <v>7245.52549</v>
+        <v>6037.93791</v>
       </c>
       <c r="BJ132" t="inlineStr">
         <is>
@@ -30306,7 +30306,7 @@
         <v>0</v>
       </c>
       <c r="BI133" t="n">
-        <v>1.05227</v>
+        <v>0.8768899999999999</v>
       </c>
       <c r="BJ133" t="inlineStr">
         <is>
@@ -30690,7 +30690,7 @@
         <v>0</v>
       </c>
       <c r="BI135" t="n">
-        <v>7244.48024</v>
+        <v>6037.06686</v>
       </c>
       <c r="BJ135" t="inlineStr">
         <is>
@@ -30866,7 +30866,7 @@
         <v>0</v>
       </c>
       <c r="BI136" t="n">
-        <v>3.86603</v>
+        <v>3.22169</v>
       </c>
       <c r="BJ136" t="inlineStr">
         <is>
@@ -31250,7 +31250,7 @@
         <v>0</v>
       </c>
       <c r="BI138" t="n">
-        <v>180.84394</v>
+        <v>150.70329</v>
       </c>
       <c r="BJ138" t="inlineStr">
         <is>
@@ -31426,7 +31426,7 @@
         <v>0</v>
       </c>
       <c r="BI139" t="n">
-        <v>0.00165</v>
+        <v>0.00138</v>
       </c>
       <c r="BJ139" t="inlineStr">
         <is>
@@ -31810,7 +31810,7 @@
         <v>0</v>
       </c>
       <c r="BI141" t="n">
-        <v>180.49688</v>
+        <v>150.41406</v>
       </c>
       <c r="BJ141" t="inlineStr">
         <is>
@@ -31986,7 +31986,7 @@
         <v>0</v>
       </c>
       <c r="BI142" t="n">
-        <v>0.00165</v>
+        <v>0.00138</v>
       </c>
       <c r="BJ142" t="inlineStr">
         <is>
@@ -32370,7 +32370,7 @@
         <v>0</v>
       </c>
       <c r="BI144" t="n">
-        <v>180.86547</v>
+        <v>150.72122</v>
       </c>
       <c r="BJ144" t="inlineStr">
         <is>
@@ -32546,7 +32546,7 @@
         <v>0</v>
       </c>
       <c r="BI145" t="n">
-        <v>0.00165</v>
+        <v>0.00138</v>
       </c>
       <c r="BJ145" t="inlineStr">
         <is>
@@ -32930,7 +32930,7 @@
         <v>0</v>
       </c>
       <c r="BI147" t="n">
-        <v>180.48729</v>
+        <v>150.40608</v>
       </c>
       <c r="BJ147" t="inlineStr">
         <is>
@@ -33106,7 +33106,7 @@
         <v>0</v>
       </c>
       <c r="BI148" t="n">
-        <v>0.34966</v>
+        <v>0.29138</v>
       </c>
       <c r="BJ148" t="inlineStr">
         <is>
@@ -33490,7 +33490,7 @@
         <v>0</v>
       </c>
       <c r="BI150" t="n">
-        <v>180.87537</v>
+        <v>150.72947</v>
       </c>
       <c r="BJ150" t="inlineStr">
         <is>
@@ -33666,7 +33666,7 @@
         <v>0</v>
       </c>
       <c r="BI151" t="n">
-        <v>0.00165</v>
+        <v>0.00138</v>
       </c>
       <c r="BJ151" t="inlineStr">
         <is>
@@ -34050,7 +34050,7 @@
         <v>0</v>
       </c>
       <c r="BI153" t="n">
-        <v>180.50665</v>
+        <v>150.4222</v>
       </c>
       <c r="BJ153" t="inlineStr">
         <is>
@@ -34226,7 +34226,7 @@
         <v>0</v>
       </c>
       <c r="BI154" t="n">
-        <v>0.00165</v>
+        <v>0.00138</v>
       </c>
       <c r="BJ154" t="inlineStr">
         <is>

</xml_diff>